<commit_message>
updated the meatadata file and added current IPSC metadata sheets
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junda-radboudumc/Radboudumc_projects/FAIRDS/fairds_storage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdaws/Downloads/fairds_storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56832FEC-E2C1-4242-B419-54DC37264490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8814D86F-9DF1-3444-8177-37F90910FC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regex" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13579" uniqueCount="2288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13612" uniqueCount="2300">
   <si>
     <t>short hand form</t>
   </si>
@@ -6680,9 +6680,6 @@
   </si>
   <si>
     <t>data processing protocol</t>
-  </si>
-  <si>
-    <t>(float)</t>
   </si>
   <si>
     <t xml:space="preserve">Weight </t>
@@ -7059,12 +7056,51 @@
   <si>
     <t>({URL}|unknown)</t>
   </si>
+  <si>
+    <t>reprogramming method</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIT_0001167</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MSIO_0000071</t>
+  </si>
+  <si>
+    <t>passage number</t>
+  </si>
+  <si>
+    <t>Manner of generation of iPSCs</t>
+  </si>
+  <si>
+    <t>episomal vectors, LV, sendai virus</t>
+  </si>
+  <si>
+    <t>P27, P52, P53</t>
+  </si>
+  <si>
+    <t>comments on changes</t>
+  </si>
+  <si>
+    <t>observation unit was DM_2</t>
+  </si>
+  <si>
+    <t>scan polarity</t>
+  </si>
+  <si>
+    <t>Relative orientation of the electromagnetic field during the selection and detection of ions in the mass spectrometer.</t>
+  </si>
+  <si>
+    <t>(positive|negative)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000465</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7130,6 +7166,10 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -7179,7 +7219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7198,6 +7238,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7504,7 +7545,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7865,10 +7906,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F765"/>
+  <dimension ref="A1:F772"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A685" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A694" sqref="A694"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A705" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B716" sqref="B716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7876,6 +7918,7 @@
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="2" width="50.5" customWidth="1"/>
     <col min="3" max="3" width="68.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16387,7 +16430,7 @@
         <v>2131</v>
       </c>
       <c r="B705" s="3" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="C705" s="6" t="s">
         <v>2204</v>
@@ -16398,7 +16441,7 @@
     </row>
     <row r="706" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A706" s="3" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="B706" s="3" t="s">
         <v>78</v>
@@ -16527,7 +16570,7 @@
         <v>2196</v>
       </c>
       <c r="B716" s="3" t="s">
-        <v>2218</v>
+        <v>55</v>
       </c>
     </row>
     <row r="717" spans="1:6" x14ac:dyDescent="0.2">
@@ -16561,592 +16604,672 @@
         <v>2153</v>
       </c>
     </row>
+    <row r="720" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A720" s="3"/>
+      <c r="B720" s="3"/>
+      <c r="C720" s="3"/>
+      <c r="F720" s="3"/>
+    </row>
     <row r="721" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A721" s="3" t="s">
-        <v>2154</v>
+      <c r="A721" t="s">
+        <v>2294</v>
       </c>
       <c r="B721" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C721" s="3" t="s">
-        <v>2155</v>
-      </c>
-      <c r="E721" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F721" s="3" t="s">
-        <v>2156</v>
+      <c r="C721" t="s">
+        <v>2295</v>
       </c>
     </row>
     <row r="722" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A722" s="3" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="B722" s="3" t="s">
-        <v>2158</v>
+        <v>241</v>
       </c>
       <c r="C722" s="3" t="s">
-        <v>2159</v>
+        <v>2155</v>
       </c>
       <c r="E722" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F722" s="3" t="s">
-        <v>2160</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="723" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A723" s="3" t="s">
-        <v>2161</v>
+        <v>2157</v>
       </c>
       <c r="B723" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C723" s="3">
-        <v>326000</v>
-      </c>
-      <c r="E723" s="3"/>
-      <c r="F723" s="3"/>
+        <v>2158</v>
+      </c>
+      <c r="C723" s="3" t="s">
+        <v>2159</v>
+      </c>
+      <c r="E723" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F723" s="3" t="s">
+        <v>2160</v>
+      </c>
     </row>
     <row r="724" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A724" s="3" t="s">
-        <v>2162</v>
+        <v>2296</v>
       </c>
       <c r="B724" s="3" t="s">
-        <v>2158</v>
+        <v>2298</v>
       </c>
       <c r="C724" s="3" t="s">
-        <v>2163</v>
-      </c>
-      <c r="E724" s="3" t="s">
-        <v>189</v>
+        <v>2224</v>
+      </c>
+      <c r="E724" s="2" t="s">
+        <v>2299</v>
       </c>
       <c r="F724" s="3" t="s">
-        <v>2164</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="725" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A725" s="3" t="s">
-        <v>2165</v>
-      </c>
-      <c r="B725" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C725" s="3">
-        <v>2</v>
-      </c>
+      <c r="A725" s="3"/>
+      <c r="B725" s="3"/>
+      <c r="C725" s="3"/>
       <c r="E725" s="3"/>
       <c r="F725" s="3"/>
     </row>
     <row r="726" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A726" s="3" t="s">
-        <v>2166</v>
+        <v>2161</v>
       </c>
       <c r="B726" s="3" t="s">
-        <v>2167</v>
-      </c>
-      <c r="C726" s="3" t="s">
-        <v>2168</v>
-      </c>
-      <c r="E726" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F726" s="3" t="s">
-        <v>2169</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C726" s="3">
+        <v>326000</v>
+      </c>
+      <c r="E726" s="3"/>
+      <c r="F726" s="3"/>
     </row>
     <row r="727" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A727" s="3" t="s">
-        <v>2170</v>
+        <v>2162</v>
       </c>
       <c r="B727" s="3" t="s">
-        <v>2216</v>
-      </c>
-      <c r="C727" s="2" t="s">
-        <v>2205</v>
-      </c>
-      <c r="E727" s="3"/>
+        <v>2158</v>
+      </c>
+      <c r="C727" s="3" t="s">
+        <v>2163</v>
+      </c>
+      <c r="E727" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="F727" s="3" t="s">
-        <v>2171</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="728" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A728" s="3" t="s">
-        <v>2172</v>
+        <v>2165</v>
       </c>
       <c r="B728" s="3" t="s">
-        <v>2167</v>
-      </c>
-      <c r="C728" s="3" t="s">
-        <v>2173</v>
-      </c>
-      <c r="E728" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F728" s="3" t="s">
-        <v>2174</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C728" s="3">
+        <v>2</v>
+      </c>
+      <c r="E728" s="3"/>
+      <c r="F728" s="3"/>
     </row>
     <row r="729" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A729" s="3" t="s">
-        <v>2175</v>
+        <v>2166</v>
       </c>
       <c r="B729" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C729" s="4">
-        <v>40909</v>
+        <v>2167</v>
+      </c>
+      <c r="C729" s="3" t="s">
+        <v>2168</v>
       </c>
       <c r="E729" s="3" t="s">
-        <v>388</v>
+        <v>189</v>
       </c>
       <c r="F729" s="3" t="s">
-        <v>2176</v>
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="730" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A730" s="3" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B730" s="3" t="s">
+        <v>2216</v>
+      </c>
+      <c r="C730" s="2" t="s">
+        <v>2205</v>
+      </c>
+      <c r="E730" s="3"/>
+      <c r="F730" s="3" t="s">
+        <v>2171</v>
       </c>
     </row>
     <row r="731" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A731" s="3" t="s">
-        <v>2177</v>
+        <v>2172</v>
       </c>
       <c r="B731" s="3" t="s">
-        <v>2158</v>
+        <v>2167</v>
       </c>
       <c r="C731" s="3" t="s">
-        <v>245</v>
+        <v>2173</v>
       </c>
       <c r="E731" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F731" s="3" t="s">
-        <v>2177</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="732" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A732" s="3" t="s">
-        <v>2178</v>
+        <v>2175</v>
       </c>
       <c r="B732" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="C732" s="3" t="s">
-        <v>245</v>
+        <v>67</v>
+      </c>
+      <c r="C732" s="4">
+        <v>40909</v>
       </c>
       <c r="E732" s="3" t="s">
-        <v>194</v>
+        <v>388</v>
       </c>
       <c r="F732" s="3" t="s">
-        <v>2179</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="733" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A733" s="3" t="s">
-        <v>2207</v>
+        <v>2290</v>
       </c>
       <c r="B733" s="3" t="s">
-        <v>2180</v>
+        <v>241</v>
       </c>
       <c r="C733" s="3" t="s">
-        <v>2181</v>
-      </c>
-      <c r="E733" s="3"/>
-      <c r="F733" s="3" t="s">
-        <v>2182</v>
-      </c>
+        <v>2293</v>
+      </c>
+      <c r="E733" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="F733" s="3"/>
     </row>
     <row r="734" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A734" s="3" t="s">
-        <v>2183</v>
+        <v>2287</v>
       </c>
       <c r="B734" s="3" t="s">
-        <v>847</v>
-      </c>
-      <c r="C734" s="3" t="s">
-        <v>1408</v>
+        <v>241</v>
+      </c>
+      <c r="C734" t="s">
+        <v>2292</v>
       </c>
       <c r="E734" s="2" t="s">
-        <v>2206</v>
+        <v>2288</v>
       </c>
       <c r="F734" s="3" t="s">
-        <v>2184</v>
-      </c>
-    </row>
-    <row r="735" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A735" s="3" t="s">
-        <v>2185</v>
-      </c>
-      <c r="B735" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C735" s="3" t="s">
-        <v>2186</v>
-      </c>
-      <c r="E735" s="3"/>
-      <c r="F735" s="3" t="s">
-        <v>2187</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="736" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A736" s="3" t="s">
-        <v>2188</v>
+        <v>2177</v>
       </c>
       <c r="B736" s="3" t="s">
-        <v>73</v>
+        <v>2158</v>
       </c>
       <c r="C736" s="3" t="s">
-        <v>2189</v>
-      </c>
-      <c r="E736" s="3"/>
+        <v>245</v>
+      </c>
+      <c r="E736" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="F736" s="3" t="s">
-        <v>2190</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="737" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A737" s="3" t="s">
-        <v>2208</v>
+        <v>2178</v>
       </c>
       <c r="B737" s="3" t="s">
-        <v>2215</v>
-      </c>
-      <c r="C737">
-        <v>1993</v>
+        <v>2158</v>
+      </c>
+      <c r="C737" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E737" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="F737" s="3" t="s">
-        <v>2208</v>
+        <v>2179</v>
+      </c>
+    </row>
+    <row r="738" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A738" s="3" t="s">
+        <v>2207</v>
+      </c>
+      <c r="B738" s="3" t="s">
+        <v>2180</v>
+      </c>
+      <c r="C738" s="3" t="s">
+        <v>2181</v>
+      </c>
+      <c r="E738" s="3"/>
+      <c r="F738" s="3" t="s">
+        <v>2182</v>
       </c>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A739" s="3" t="s">
-        <v>2209</v>
+        <v>2183</v>
       </c>
       <c r="B739" s="3" t="s">
-        <v>10</v>
+        <v>847</v>
       </c>
       <c r="C739" s="3" t="s">
-        <v>2210</v>
+        <v>1408</v>
+      </c>
+      <c r="E739" s="2" t="s">
+        <v>2206</v>
+      </c>
+      <c r="F739" s="3" t="s">
+        <v>2184</v>
       </c>
     </row>
     <row r="740" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A740" s="3" t="s">
-        <v>2211</v>
+        <v>2185</v>
       </c>
       <c r="B740" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C740">
-        <v>25</v>
+        <v>2216</v>
+      </c>
+      <c r="C740" s="3" t="s">
+        <v>2186</v>
+      </c>
+      <c r="E740" s="3"/>
+      <c r="F740" s="3" t="s">
+        <v>2187</v>
       </c>
     </row>
     <row r="741" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A741" s="3" t="s">
-        <v>2212</v>
+        <v>2188</v>
       </c>
       <c r="B741" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C741" t="s">
-        <v>2213</v>
-      </c>
-      <c r="F741" t="s">
-        <v>2214</v>
-      </c>
-    </row>
-    <row r="743" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A743" s="3" t="s">
-        <v>2217</v>
-      </c>
-      <c r="B743" s="3" t="s">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="C741" s="3" t="s">
+        <v>2189</v>
+      </c>
+      <c r="E741" s="3"/>
+      <c r="F741" s="3" t="s">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="742" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A742" s="3" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B742" s="3" t="s">
+        <v>2215</v>
+      </c>
+      <c r="C742">
+        <v>1993</v>
+      </c>
+      <c r="F742" s="3" t="s">
+        <v>2208</v>
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A744" s="3" t="s">
-        <v>2220</v>
+        <v>2209</v>
       </c>
       <c r="B744" s="3" t="s">
-        <v>2222</v>
-      </c>
-      <c r="C744" t="s">
-        <v>2224</v>
+        <v>10</v>
+      </c>
+      <c r="C744" s="3" t="s">
+        <v>2210</v>
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A745" s="3" t="s">
-        <v>2264</v>
+        <v>2211</v>
       </c>
       <c r="B745" s="3" t="s">
-        <v>2279</v>
+        <v>28</v>
+      </c>
+      <c r="C745">
+        <v>25</v>
       </c>
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A746" s="3" t="s">
-        <v>2265</v>
+        <v>2212</v>
       </c>
       <c r="B746" s="3" t="s">
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="747" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A747" s="3" t="s">
-        <v>2221</v>
-      </c>
-      <c r="B747" s="3" t="s">
-        <v>2223</v>
-      </c>
-      <c r="C747" t="s">
-        <v>2225</v>
-      </c>
-    </row>
-    <row r="748" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C746" t="s">
+        <v>2213</v>
+      </c>
+      <c r="F746" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="748" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A748" s="3" t="s">
-        <v>2266</v>
+        <v>2217</v>
       </c>
       <c r="B748" s="3" t="s">
-        <v>2278</v>
-      </c>
-      <c r="E748" s="15" t="s">
-        <v>2267</v>
+        <v>10</v>
       </c>
     </row>
     <row r="749" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A749" s="3" t="s">
-        <v>2226</v>
+        <v>2219</v>
       </c>
       <c r="B749" s="3" t="s">
-        <v>50</v>
+        <v>2221</v>
+      </c>
+      <c r="C749" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="750" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A750" s="3" t="s">
+        <v>2263</v>
+      </c>
+      <c r="B750" s="3" t="s">
+        <v>2278</v>
       </c>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A751" s="3" t="s">
-        <v>2228</v>
+        <v>2264</v>
       </c>
       <c r="B751" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C751" t="s">
-        <v>2260</v>
-      </c>
-      <c r="E751" s="12" t="s">
-        <v>2261</v>
-      </c>
-      <c r="F751" t="s">
-        <v>2229</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="752" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A752" s="3" t="s">
-        <v>2230</v>
+        <v>2220</v>
       </c>
       <c r="B752" s="3" t="s">
+        <v>2222</v>
+      </c>
+      <c r="C752" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A753" s="3" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B753" s="3" t="s">
+        <v>2277</v>
+      </c>
+      <c r="E753" s="15" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="754" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A754" s="3" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B754" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="756" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A756" s="3" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B756" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="753" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A753" s="3" t="s">
+      <c r="C756" t="s">
+        <v>2259</v>
+      </c>
+      <c r="E756" s="12" t="s">
+        <v>2260</v>
+      </c>
+      <c r="F756" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="757" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A757" s="3" t="s">
+        <v>2229</v>
+      </c>
+      <c r="B757" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="758" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A758" s="3" t="s">
+        <v>2231</v>
+      </c>
+      <c r="B758" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C758" t="s">
+        <v>1231</v>
+      </c>
+      <c r="E758" t="s">
         <v>2232</v>
-      </c>
-      <c r="B753" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C753" t="s">
-        <v>1231</v>
-      </c>
-      <c r="E753" t="s">
-        <v>2233</v>
-      </c>
-    </row>
-    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A755" s="10" t="s">
-        <v>2262</v>
-      </c>
-      <c r="B755" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C755" s="13" t="s">
-        <v>2256</v>
-      </c>
-      <c r="E755" s="12" t="s">
-        <v>2268</v>
-      </c>
-      <c r="F755" s="11" t="s">
-        <v>2245</v>
-      </c>
-    </row>
-    <row r="756" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A756" s="10" t="s">
-        <v>2235</v>
-      </c>
-      <c r="B756" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C756" s="13" t="s">
-        <v>2257</v>
-      </c>
-      <c r="E756" s="12" t="s">
-        <v>2277</v>
-      </c>
-      <c r="F756" t="s">
-        <v>2246</v>
-      </c>
-    </row>
-    <row r="757" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A757" s="10" t="s">
-        <v>2236</v>
-      </c>
-      <c r="B757" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C757" s="13" t="s">
-        <v>2258</v>
-      </c>
-      <c r="E757" s="12" t="s">
-        <v>2276</v>
-      </c>
-      <c r="F757" t="s">
-        <v>2247</v>
-      </c>
-    </row>
-    <row r="758" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A758" s="10" t="s">
-        <v>2237</v>
-      </c>
-      <c r="B758" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C758" s="13" t="s">
-        <v>2259</v>
-      </c>
-      <c r="E758" s="12" t="s">
-        <v>2271</v>
-      </c>
-      <c r="F758" t="s">
-        <v>2248</v>
-      </c>
-    </row>
-    <row r="759" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A759" s="10" t="s">
-        <v>2238</v>
-      </c>
-      <c r="B759" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C759" s="13" t="s">
-        <v>2281</v>
-      </c>
-      <c r="E759" s="12" t="s">
-        <v>2269</v>
-      </c>
-      <c r="F759" t="s">
-        <v>2249</v>
       </c>
     </row>
     <row r="760" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A760" s="10" t="s">
-        <v>2239</v>
+        <v>2261</v>
       </c>
       <c r="B760" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C760" s="13" t="s">
-        <v>2282</v>
+        <v>2255</v>
       </c>
       <c r="E760" s="12" t="s">
-        <v>2270</v>
-      </c>
-      <c r="F760" t="s">
-        <v>2250</v>
+        <v>2267</v>
+      </c>
+      <c r="F760" s="11" t="s">
+        <v>2244</v>
       </c>
     </row>
     <row r="761" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A761" s="10" t="s">
-        <v>2240</v>
+        <v>2234</v>
       </c>
       <c r="B761" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C761" s="13" t="s">
-        <v>2283</v>
+        <v>2256</v>
       </c>
       <c r="E761" s="12" t="s">
-        <v>2273</v>
+        <v>2276</v>
       </c>
       <c r="F761" t="s">
-        <v>2251</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="762" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A762" s="10" t="s">
-        <v>2241</v>
+        <v>2235</v>
       </c>
       <c r="B762" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C762" s="13" t="s">
-        <v>2284</v>
+        <v>2257</v>
       </c>
       <c r="E762" s="12" t="s">
-        <v>2274</v>
+        <v>2275</v>
       </c>
       <c r="F762" t="s">
-        <v>2252</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="763" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A763" s="10" t="s">
-        <v>2242</v>
+        <v>2236</v>
       </c>
       <c r="B763" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C763" s="13" t="s">
-        <v>2285</v>
-      </c>
-      <c r="E763" s="12"/>
+        <v>2258</v>
+      </c>
+      <c r="E763" s="12" t="s">
+        <v>2270</v>
+      </c>
       <c r="F763" t="s">
-        <v>2253</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="764" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A764" s="10" t="s">
-        <v>2243</v>
+        <v>2237</v>
       </c>
       <c r="B764" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C764" s="13" t="s">
-        <v>2286</v>
+        <v>2280</v>
       </c>
       <c r="E764" s="12" t="s">
-        <v>2275</v>
+        <v>2268</v>
       </c>
       <c r="F764" t="s">
-        <v>2254</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="765" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A765" s="10" t="s">
-        <v>2244</v>
+        <v>2238</v>
       </c>
       <c r="B765" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C765" s="13" t="s">
-        <v>2257</v>
+        <v>2281</v>
       </c>
       <c r="E765" s="12" t="s">
+        <v>2269</v>
+      </c>
+      <c r="F765" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="766" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A766" s="10" t="s">
+        <v>2239</v>
+      </c>
+      <c r="B766" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C766" s="13" t="s">
+        <v>2282</v>
+      </c>
+      <c r="E766" s="12" t="s">
         <v>2272</v>
       </c>
-      <c r="F765" t="s">
-        <v>2255</v>
-      </c>
+      <c r="F766" t="s">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="767" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A767" s="10" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B767" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C767" s="13" t="s">
+        <v>2283</v>
+      </c>
+      <c r="E767" s="12" t="s">
+        <v>2273</v>
+      </c>
+      <c r="F767" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="768" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A768" s="10" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B768" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C768" s="13" t="s">
+        <v>2284</v>
+      </c>
+      <c r="E768" s="12"/>
+      <c r="F768" t="s">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="769" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A769" s="10" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B769" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C769" s="13" t="s">
+        <v>2285</v>
+      </c>
+      <c r="E769" s="12" t="s">
+        <v>2274</v>
+      </c>
+      <c r="F769" t="s">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="770" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A770" s="10" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B770" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C770" s="13" t="s">
+        <v>2256</v>
+      </c>
+      <c r="E770" s="12" t="s">
+        <v>2271</v>
+      </c>
+      <c r="F770" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A772" s="10"/>
+      <c r="B772" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E11" r:id="rId1" display="https://w3id.org/mixs/terms/0000018" xr:uid="{E5B9998C-031F-4241-A1E7-C7E6D8677047}"/>
     <hyperlink ref="E559" r:id="rId2" xr:uid="{EC998EC6-084C-3048-AC10-E9220B7375C6}"/>
-    <hyperlink ref="C727" r:id="rId3" xr:uid="{52CD8FE2-FCDC-D545-943E-8E5695A7E4C6}"/>
-    <hyperlink ref="E734" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
-    <hyperlink ref="E751" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
+    <hyperlink ref="C730" r:id="rId3" xr:uid="{52CD8FE2-FCDC-D545-943E-8E5695A7E4C6}"/>
+    <hyperlink ref="E739" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
+    <hyperlink ref="E756" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
+    <hyperlink ref="E734" r:id="rId6" xr:uid="{02045287-A2C1-2246-9C9A-09E35261DF8C}"/>
+    <hyperlink ref="E733" r:id="rId7" xr:uid="{0FD7D99F-B07A-9643-9AD4-E0FEFB759009}"/>
+    <hyperlink ref="E724" r:id="rId8" xr:uid="{383BC27E-9C9C-494A-88BF-6F6240C62D83}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -17157,7 +17280,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -17553,7 +17678,7 @@
         <v>1718</v>
       </c>
       <c r="C12" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D12" t="s">
         <v>1719</v>
@@ -17567,7 +17692,7 @@
         <v>1718</v>
       </c>
       <c r="C13" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="D13" t="s">
         <v>1719</v>
@@ -17581,7 +17706,7 @@
         <v>1718</v>
       </c>
       <c r="C14" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
       <c r="D14" t="s">
         <v>1719</v>
@@ -17595,7 +17720,7 @@
         <v>1718</v>
       </c>
       <c r="C15" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="D15" t="s">
         <v>1719</v>
@@ -17609,7 +17734,7 @@
         <v>1718</v>
       </c>
       <c r="C16" t="s">
-        <v>2265</v>
+        <v>2264</v>
       </c>
       <c r="D16" t="s">
         <v>1719</v>
@@ -17637,7 +17762,7 @@
         <v>1718</v>
       </c>
       <c r="C18" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="D18" t="s">
         <v>1719</v>
@@ -17665,13 +17790,13 @@
         <v>1718</v>
       </c>
       <c r="C20" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
       <c r="D20" t="s">
         <v>1715</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -17682,13 +17807,13 @@
         <v>1718</v>
       </c>
       <c r="C21" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="D21" t="s">
         <v>1715</v>
       </c>
       <c r="G21" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -17699,13 +17824,13 @@
         <v>1718</v>
       </c>
       <c r="C22" t="s">
-        <v>2236</v>
+        <v>2235</v>
       </c>
       <c r="D22" t="s">
         <v>1715</v>
       </c>
       <c r="G22" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -17716,13 +17841,13 @@
         <v>1718</v>
       </c>
       <c r="C23" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="D23" t="s">
         <v>1715</v>
       </c>
       <c r="G23" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -17733,13 +17858,13 @@
         <v>1718</v>
       </c>
       <c r="C24" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="D24" t="s">
         <v>1715</v>
       </c>
       <c r="G24" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -17750,13 +17875,13 @@
         <v>1718</v>
       </c>
       <c r="C25" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="D25" t="s">
         <v>1715</v>
       </c>
       <c r="G25" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -17767,13 +17892,13 @@
         <v>1718</v>
       </c>
       <c r="C26" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="D26" t="s">
         <v>1715</v>
       </c>
       <c r="G26" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -17784,13 +17909,13 @@
         <v>1718</v>
       </c>
       <c r="C27" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="D27" t="s">
         <v>1715</v>
       </c>
       <c r="G27" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -17801,13 +17926,13 @@
         <v>1718</v>
       </c>
       <c r="C28" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="D28" t="s">
         <v>1715</v>
       </c>
       <c r="G28" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -17818,13 +17943,13 @@
         <v>1718</v>
       </c>
       <c r="C29" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="D29" t="s">
         <v>1715</v>
       </c>
       <c r="G29" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -17835,13 +17960,13 @@
         <v>1718</v>
       </c>
       <c r="C30" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="D30" t="s">
         <v>1715</v>
       </c>
       <c r="G30" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -17992,10 +18117,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D2456"/>
+  <dimension ref="A1:D2459"/>
   <sheetViews>
-    <sheetView topLeftCell="A2406" workbookViewId="0">
-      <selection activeCell="C2450" sqref="C2450"/>
+    <sheetView topLeftCell="A2413" workbookViewId="0">
+      <selection activeCell="C2456" sqref="C2456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -51913,16 +52038,16 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="2425" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2426" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2425" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2426" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2426" t="s">
         <v>1720</v>
       </c>
-      <c r="B2426" s="3" t="s">
+      <c r="B2426" t="s">
         <v>2192</v>
       </c>
-      <c r="C2426" s="3" t="s">
-        <v>2154</v>
+      <c r="C2426" t="s">
+        <v>2294</v>
       </c>
       <c r="D2426" t="s">
         <v>1719</v>
@@ -51936,10 +52061,10 @@
         <v>2192</v>
       </c>
       <c r="C2427" s="3" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="D2427" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="2428" spans="1:4" x14ac:dyDescent="0.2">
@@ -51950,10 +52075,10 @@
         <v>2192</v>
       </c>
       <c r="C2428" s="3" t="s">
-        <v>2161</v>
+        <v>2157</v>
       </c>
       <c r="D2428" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="2429" spans="1:4" x14ac:dyDescent="0.2">
@@ -51964,10 +52089,10 @@
         <v>2192</v>
       </c>
       <c r="C2429" s="3" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="D2429" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="2430" spans="1:4" x14ac:dyDescent="0.2">
@@ -51978,10 +52103,10 @@
         <v>2192</v>
       </c>
       <c r="C2430" s="3" t="s">
-        <v>2165</v>
+        <v>2162</v>
       </c>
       <c r="D2430" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="2431" spans="1:4" x14ac:dyDescent="0.2">
@@ -51992,10 +52117,10 @@
         <v>2192</v>
       </c>
       <c r="C2431" s="3" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="D2431" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="2432" spans="1:4" x14ac:dyDescent="0.2">
@@ -52006,10 +52131,10 @@
         <v>2192</v>
       </c>
       <c r="C2432" s="3" t="s">
-        <v>1557</v>
+        <v>2166</v>
       </c>
       <c r="D2432" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="2433" spans="1:4" x14ac:dyDescent="0.2">
@@ -52020,7 +52145,7 @@
         <v>2192</v>
       </c>
       <c r="C2433" s="3" t="s">
-        <v>2170</v>
+        <v>1557</v>
       </c>
       <c r="D2433" t="s">
         <v>1719</v>
@@ -52034,7 +52159,7 @@
         <v>2192</v>
       </c>
       <c r="C2434" s="3" t="s">
-        <v>2172</v>
+        <v>2170</v>
       </c>
       <c r="D2434" t="s">
         <v>1719</v>
@@ -52048,7 +52173,7 @@
         <v>2192</v>
       </c>
       <c r="C2435" s="3" t="s">
-        <v>2175</v>
+        <v>2172</v>
       </c>
       <c r="D2435" t="s">
         <v>1719</v>
@@ -52062,7 +52187,7 @@
         <v>2192</v>
       </c>
       <c r="C2436" s="3" t="s">
-        <v>2209</v>
+        <v>2175</v>
       </c>
       <c r="D2436" t="s">
         <v>1719</v>
@@ -52076,10 +52201,10 @@
         <v>2192</v>
       </c>
       <c r="C2437" s="3" t="s">
-        <v>2211</v>
+        <v>2209</v>
       </c>
       <c r="D2437" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="2438" spans="1:4" x14ac:dyDescent="0.2">
@@ -52090,7 +52215,7 @@
         <v>2192</v>
       </c>
       <c r="C2438" s="3" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="D2438" t="s">
         <v>1714</v>
@@ -52104,24 +52229,38 @@
         <v>2192</v>
       </c>
       <c r="C2439" s="3" t="s">
-        <v>1152</v>
+        <v>2212</v>
       </c>
       <c r="D2439" t="s">
         <v>1714</v>
       </c>
     </row>
+    <row r="2440" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2440" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B2440" s="3" t="s">
+        <v>2192</v>
+      </c>
+      <c r="C2440" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D2440" t="s">
+        <v>1714</v>
+      </c>
+    </row>
     <row r="2441" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2441" t="s">
         <v>1720</v>
       </c>
       <c r="B2441" s="3" t="s">
-        <v>2227</v>
-      </c>
-      <c r="C2441" s="3" t="s">
-        <v>2228</v>
+        <v>2192</v>
+      </c>
+      <c r="C2441" s="16" t="s">
+        <v>2290</v>
       </c>
       <c r="D2441" t="s">
-        <v>1715</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="2442" spans="1:4" x14ac:dyDescent="0.2">
@@ -52129,37 +52268,60 @@
         <v>1720</v>
       </c>
       <c r="B2442" s="3" t="s">
+        <v>2192</v>
+      </c>
+      <c r="C2442" s="3" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D2442" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2443" s="3"/>
+      <c r="C2443" s="3"/>
+    </row>
+    <row r="2444" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2444" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B2444" s="3" t="s">
+        <v>2226</v>
+      </c>
+      <c r="C2444" s="3" t="s">
         <v>2227</v>
       </c>
-      <c r="C2442" s="3" t="s">
-        <v>2230</v>
-      </c>
-      <c r="D2442" t="s">
-        <v>1715</v>
-      </c>
-    </row>
-    <row r="2443" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2443" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B2443" s="3" t="s">
-        <v>2227</v>
-      </c>
-      <c r="C2443" s="3" t="s">
-        <v>2232</v>
-      </c>
-      <c r="D2443" t="s">
-        <v>1715</v>
-      </c>
-    </row>
-    <row r="2444" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2444" s="3"/>
+      <c r="D2444" t="s">
+        <v>1715</v>
+      </c>
     </row>
     <row r="2445" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2445" s="3"/>
+      <c r="A2445" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B2445" s="3" t="s">
+        <v>2226</v>
+      </c>
+      <c r="C2445" s="3" t="s">
+        <v>2229</v>
+      </c>
+      <c r="D2445" t="s">
+        <v>1715</v>
+      </c>
     </row>
     <row r="2446" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2446" s="3"/>
+      <c r="A2446" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B2446" s="3" t="s">
+        <v>2226</v>
+      </c>
+      <c r="C2446" s="3" t="s">
+        <v>2231</v>
+      </c>
+      <c r="D2446" t="s">
+        <v>1715</v>
+      </c>
     </row>
     <row r="2447" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2447" s="3"/>
@@ -52190,6 +52352,15 @@
     </row>
     <row r="2456" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2456" s="3"/>
+    </row>
+    <row r="2457" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2457" s="3"/>
+    </row>
+    <row r="2458" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2458" s="3"/>
+    </row>
+    <row r="2459" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2459" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -52199,10 +52370,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D254"/>
+  <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53479,7 +53650,7 @@
         <v>2193</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>1714</v>
@@ -53694,7 +53865,7 @@
         <v>2194</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>1714</v>
@@ -54049,7 +54220,7 @@
         <v>2195</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>1714</v>
@@ -54278,7 +54449,7 @@
         <v>2197</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>1714</v>
@@ -54535,7 +54706,7 @@
         <v>2198</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>1714</v>
@@ -54549,7 +54720,7 @@
         <v>2198</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>2134</v>
+        <v>2296</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>1714</v>
@@ -54563,10 +54734,10 @@
         <v>2198</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -54577,30 +54748,30 @@
         <v>2198</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>2217</v>
+        <v>2136</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>1719</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B186" s="3"/>
-      <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
+      <c r="A186" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>2198</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>2217</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>1719</v>
+      </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>2199</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>2104</v>
-      </c>
-      <c r="D187" s="3" t="s">
-        <v>1714</v>
-      </c>
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
@@ -54610,10 +54781,10 @@
         <v>2199</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -54624,7 +54795,7 @@
         <v>2199</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>1715</v>
@@ -54638,7 +54809,7 @@
         <v>2199</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>1715</v>
@@ -54652,7 +54823,7 @@
         <v>2199</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>1715</v>
@@ -54666,10 +54837,10 @@
         <v>2199</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D192" s="9" t="s">
-        <v>1714</v>
+        <v>2113</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -54680,7 +54851,7 @@
         <v>2199</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>1714</v>
@@ -54694,9 +54865,9 @@
         <v>2199</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="D194" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D194" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -54708,7 +54879,7 @@
         <v>2199</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>1714</v>
@@ -54722,7 +54893,7 @@
         <v>2199</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>2150</v>
+        <v>2122</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>1714</v>
@@ -54736,10 +54907,10 @@
         <v>2199</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>2152</v>
+        <v>2150</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -54750,10 +54921,10 @@
         <v>2199</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>2131</v>
+        <v>2152</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -54763,8 +54934,8 @@
       <c r="B199" s="3" t="s">
         <v>2199</v>
       </c>
-      <c r="C199" s="9" t="s">
-        <v>2231</v>
+      <c r="C199" s="3" t="s">
+        <v>2131</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>1714</v>
@@ -54777,8 +54948,8 @@
       <c r="B200" s="3" t="s">
         <v>2199</v>
       </c>
-      <c r="C200" s="3" t="s">
-        <v>2134</v>
+      <c r="C200" s="9" t="s">
+        <v>2230</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>1714</v>
@@ -54792,10 +54963,10 @@
         <v>2199</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -54806,30 +54977,30 @@
         <v>2199</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>2217</v>
+        <v>2136</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>1719</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B203" s="3"/>
-      <c r="C203" s="3"/>
-      <c r="D203" s="3"/>
+      <c r="A203" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>2199</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>2217</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>1719</v>
+      </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>2201</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>1714</v>
-      </c>
+      <c r="B204" s="3"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
@@ -54839,10 +55010,10 @@
         <v>2200</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>2106</v>
+        <v>2201</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -54853,7 +55024,7 @@
         <v>2200</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>1715</v>
@@ -54867,7 +55038,7 @@
         <v>2200</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>1715</v>
@@ -54881,7 +55052,7 @@
         <v>2200</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>1715</v>
@@ -54895,10 +55066,10 @@
         <v>2200</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D209" s="9" t="s">
-        <v>1714</v>
+        <v>2113</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -54909,7 +55080,7 @@
         <v>2200</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="D210" s="9" t="s">
         <v>1714</v>
@@ -54923,9 +55094,9 @@
         <v>2200</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="D211" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D211" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -54937,7 +55108,7 @@
         <v>2200</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>1714</v>
@@ -54951,7 +55122,7 @@
         <v>2200</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>2131</v>
+        <v>2122</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>1714</v>
@@ -54964,8 +55135,8 @@
       <c r="B214" s="3" t="s">
         <v>2200</v>
       </c>
-      <c r="C214" s="9" t="s">
-        <v>2231</v>
+      <c r="C214" s="3" t="s">
+        <v>2131</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>1714</v>
@@ -54978,8 +55149,8 @@
       <c r="B215" s="3" t="s">
         <v>2200</v>
       </c>
-      <c r="C215" s="3" t="s">
-        <v>2134</v>
+      <c r="C215" s="9" t="s">
+        <v>2230</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>1714</v>
@@ -54993,30 +55164,30 @@
         <v>2200</v>
       </c>
       <c r="C216" s="3" t="s">
+        <v>2134</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>2200</v>
+      </c>
+      <c r="C217" s="3" t="s">
         <v>2136</v>
       </c>
-      <c r="D216" s="3" t="s">
+      <c r="D217" s="3" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B217" s="3"/>
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
-    </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>2202</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>2201</v>
-      </c>
-      <c r="D218" s="3" t="s">
-        <v>1714</v>
-      </c>
+      <c r="B218" s="3"/>
+      <c r="C218" s="3"/>
+      <c r="D218" s="3"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
@@ -55026,10 +55197,10 @@
         <v>2202</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>2106</v>
+        <v>2201</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -55040,7 +55211,7 @@
         <v>2202</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>1715</v>
@@ -55054,7 +55225,7 @@
         <v>2202</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>1715</v>
@@ -55068,7 +55239,7 @@
         <v>2202</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>1715</v>
@@ -55082,10 +55253,10 @@
         <v>2202</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D223" s="9" t="s">
-        <v>1714</v>
+        <v>2113</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -55096,7 +55267,7 @@
         <v>2202</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="D224" s="9" t="s">
         <v>1714</v>
@@ -55110,9 +55281,9 @@
         <v>2202</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="D225" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D225" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55124,7 +55295,7 @@
         <v>2202</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>1714</v>
@@ -55138,7 +55309,7 @@
         <v>2202</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>2150</v>
+        <v>2122</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>1714</v>
@@ -55152,10 +55323,10 @@
         <v>2202</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>2152</v>
+        <v>2150</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -55166,10 +55337,10 @@
         <v>2202</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>2131</v>
+        <v>2152</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -55179,8 +55350,8 @@
       <c r="B230" s="3" t="s">
         <v>2202</v>
       </c>
-      <c r="C230" s="9" t="s">
-        <v>2231</v>
+      <c r="C230" s="3" t="s">
+        <v>2131</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>1714</v>
@@ -55193,8 +55364,8 @@
       <c r="B231" s="3" t="s">
         <v>2202</v>
       </c>
-      <c r="C231" s="3" t="s">
-        <v>2134</v>
+      <c r="C231" s="9" t="s">
+        <v>2230</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>1714</v>
@@ -55208,10 +55379,10 @@
         <v>2202</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -55222,24 +55393,24 @@
         <v>2202</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>2217</v>
+        <v>2136</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" s="14" t="s">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
         <v>1774</v>
       </c>
-      <c r="B235" s="14" t="s">
-        <v>2263</v>
-      </c>
-      <c r="C235" s="14" t="s">
-        <v>2104</v>
-      </c>
-      <c r="D235" s="14" t="s">
-        <v>1714</v>
+      <c r="B234" s="3" t="s">
+        <v>2202</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>2217</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -55247,13 +55418,13 @@
         <v>1774</v>
       </c>
       <c r="B236" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C236" s="14" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
       <c r="D236" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -55261,10 +55432,10 @@
         <v>1774</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="D237" s="14" t="s">
         <v>1715</v>
@@ -55275,10 +55446,10 @@
         <v>1774</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C238" s="14" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="D238" s="14" t="s">
         <v>1715</v>
@@ -55289,10 +55460,10 @@
         <v>1774</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C239" s="14" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="D239" s="14" t="s">
         <v>1715</v>
@@ -55303,13 +55474,13 @@
         <v>1774</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -55317,10 +55488,10 @@
         <v>1774</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="D241" s="14" t="s">
         <v>1714</v>
@@ -55331,10 +55502,10 @@
         <v>1774</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
       <c r="D242" s="14" t="s">
         <v>1714</v>
@@ -55345,10 +55516,10 @@
         <v>1774</v>
       </c>
       <c r="B243" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="D243" s="14" t="s">
         <v>1714</v>
@@ -55359,10 +55530,10 @@
         <v>1774</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>2140</v>
+        <v>2122</v>
       </c>
       <c r="D244" s="14" t="s">
         <v>1714</v>
@@ -55373,10 +55544,10 @@
         <v>1774</v>
       </c>
       <c r="B245" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
       <c r="D245" s="14" t="s">
         <v>1714</v>
@@ -55387,13 +55558,13 @@
         <v>1774</v>
       </c>
       <c r="B246" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C246" s="14" t="s">
-        <v>2146</v>
-      </c>
-      <c r="D246" s="9" t="s">
-        <v>1719</v>
+        <v>2142</v>
+      </c>
+      <c r="D246" s="14" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
@@ -55401,10 +55572,10 @@
         <v>1774</v>
       </c>
       <c r="B247" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C247" s="14" t="s">
-        <v>2148</v>
+        <v>2146</v>
       </c>
       <c r="D247" s="9" t="s">
         <v>1719</v>
@@ -55415,13 +55586,13 @@
         <v>1774</v>
       </c>
       <c r="B248" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C248" s="14" t="s">
-        <v>2138</v>
-      </c>
-      <c r="D248" s="14" t="s">
-        <v>1715</v>
+        <v>2148</v>
+      </c>
+      <c r="D248" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -55429,10 +55600,10 @@
         <v>1774</v>
       </c>
       <c r="B249" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C249" s="14" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="D249" s="14" t="s">
         <v>1715</v>
@@ -55443,13 +55614,13 @@
         <v>1774</v>
       </c>
       <c r="B250" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C250" s="14" t="s">
-        <v>2131</v>
+        <v>2139</v>
       </c>
       <c r="D250" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
@@ -55457,10 +55628,10 @@
         <v>1774</v>
       </c>
       <c r="B251" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C251" s="14" t="s">
-        <v>2231</v>
+        <v>2131</v>
       </c>
       <c r="D251" s="14" t="s">
         <v>1714</v>
@@ -55471,10 +55642,10 @@
         <v>1774</v>
       </c>
       <c r="B252" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C252" s="14" t="s">
-        <v>2134</v>
+        <v>2230</v>
       </c>
       <c r="D252" s="14" t="s">
         <v>1714</v>
@@ -55485,13 +55656,13 @@
         <v>1774</v>
       </c>
       <c r="B253" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C253" s="14" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="D253" s="14" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
@@ -55499,12 +55670,26 @@
         <v>1774</v>
       </c>
       <c r="B254" s="14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="C254" s="14" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D254" s="14" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B255" s="14" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C255" s="14" t="s">
         <v>2217</v>
       </c>
-      <c r="D254" s="14" t="s">
+      <c r="D255" s="14" t="s">
         <v>1719</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new fields to 'Observation Unit' and 'metabolomics_T'
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdaws/Downloads/fairds_storage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdaws/Documents/FAIRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8814D86F-9DF1-3444-8177-37F90910FC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9064C0B-8CD0-864F-B586-EEB5B2D1CB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regex" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13612" uniqueCount="2300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13642" uniqueCount="2305">
   <si>
     <t>short hand form</t>
   </si>
@@ -7094,6 +7094,21 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/MS_1000465</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>additional data processing protocol</t>
+  </si>
+  <si>
+    <t>labnotes as pdf</t>
+  </si>
+  <si>
+    <t>fitzpatrick</t>
   </si>
 </sst>
 </file>
@@ -7906,11 +7921,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F772"/>
+  <dimension ref="A1:F778"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A705" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B716" sqref="B716"/>
+    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A737" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B739" sqref="B739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16820,444 +16835,500 @@
         <v>2291</v>
       </c>
     </row>
+    <row r="735" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A735" s="3" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B735" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E735" s="2"/>
+      <c r="F735" s="3"/>
+    </row>
     <row r="736" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A736" s="3" t="s">
-        <v>2177</v>
+        <v>2301</v>
       </c>
       <c r="B736" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="C736" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E736" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F736" s="3" t="s">
-        <v>2177</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="E736" s="2"/>
+      <c r="F736" s="3"/>
     </row>
     <row r="737" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A737" s="3" t="s">
-        <v>2178</v>
+        <v>2304</v>
       </c>
       <c r="B737" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="C737" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E737" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F737" s="3" t="s">
-        <v>2179</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E737" s="2"/>
+      <c r="F737" s="3"/>
     </row>
     <row r="738" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A738" s="3" t="s">
-        <v>2207</v>
+        <v>2302</v>
       </c>
       <c r="B738" s="3" t="s">
-        <v>2180</v>
-      </c>
-      <c r="C738" s="3" t="s">
-        <v>2181</v>
-      </c>
-      <c r="E738" s="3"/>
-      <c r="F738" s="3" t="s">
-        <v>2182</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E738" s="2"/>
+      <c r="F738" s="3"/>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A739" s="3" t="s">
-        <v>2183</v>
+        <v>2303</v>
       </c>
       <c r="B739" s="3" t="s">
-        <v>847</v>
-      </c>
-      <c r="C739" s="3" t="s">
-        <v>1408</v>
-      </c>
-      <c r="E739" s="2" t="s">
-        <v>2206</v>
-      </c>
-      <c r="F739" s="3" t="s">
-        <v>2184</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="E739" s="2"/>
+      <c r="F739" s="3"/>
     </row>
     <row r="740" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A740" s="3" t="s">
-        <v>2185</v>
-      </c>
-      <c r="B740" s="3" t="s">
-        <v>2216</v>
-      </c>
-      <c r="C740" s="3" t="s">
-        <v>2186</v>
-      </c>
-      <c r="E740" s="3"/>
-      <c r="F740" s="3" t="s">
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="741" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A741" s="3" t="s">
-        <v>2188</v>
-      </c>
-      <c r="B741" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C741" s="3" t="s">
-        <v>2189</v>
-      </c>
-      <c r="E741" s="3"/>
-      <c r="F741" s="3" t="s">
-        <v>2190</v>
-      </c>
+      <c r="A740" s="3"/>
+      <c r="B740" s="3"/>
+      <c r="E740" s="2"/>
+      <c r="F740" s="3"/>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A742" s="3" t="s">
-        <v>2208</v>
+        <v>2177</v>
       </c>
       <c r="B742" s="3" t="s">
-        <v>2215</v>
-      </c>
-      <c r="C742">
-        <v>1993</v>
+        <v>2158</v>
+      </c>
+      <c r="C742" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E742" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="F742" s="3" t="s">
-        <v>2208</v>
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="743" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A743" s="3" t="s">
+        <v>2178</v>
+      </c>
+      <c r="B743" s="3" t="s">
+        <v>2158</v>
+      </c>
+      <c r="C743" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E743" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F743" s="3" t="s">
+        <v>2179</v>
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A744" s="3" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="B744" s="3" t="s">
-        <v>10</v>
+        <v>2180</v>
       </c>
       <c r="C744" s="3" t="s">
-        <v>2210</v>
+        <v>2181</v>
+      </c>
+      <c r="E744" s="3"/>
+      <c r="F744" s="3" t="s">
+        <v>2182</v>
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A745" s="3" t="s">
-        <v>2211</v>
+        <v>2183</v>
       </c>
       <c r="B745" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C745">
-        <v>25</v>
+        <v>847</v>
+      </c>
+      <c r="C745" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E745" s="2" t="s">
+        <v>2206</v>
+      </c>
+      <c r="F745" s="3" t="s">
+        <v>2184</v>
       </c>
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A746" s="3" t="s">
-        <v>2212</v>
+        <v>2185</v>
       </c>
       <c r="B746" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C746" t="s">
-        <v>2213</v>
-      </c>
-      <c r="F746" t="s">
-        <v>2214</v>
+        <v>2216</v>
+      </c>
+      <c r="C746" s="3" t="s">
+        <v>2186</v>
+      </c>
+      <c r="E746" s="3"/>
+      <c r="F746" s="3" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="747" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A747" s="3" t="s">
+        <v>2188</v>
+      </c>
+      <c r="B747" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C747" s="3" t="s">
+        <v>2189</v>
+      </c>
+      <c r="E747" s="3"/>
+      <c r="F747" s="3" t="s">
+        <v>2190</v>
       </c>
     </row>
     <row r="748" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A748" s="3" t="s">
-        <v>2217</v>
+        <v>2208</v>
       </c>
       <c r="B748" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="749" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A749" s="3" t="s">
-        <v>2219</v>
-      </c>
-      <c r="B749" s="3" t="s">
-        <v>2221</v>
-      </c>
-      <c r="C749" t="s">
-        <v>2223</v>
+        <v>2215</v>
+      </c>
+      <c r="C748">
+        <v>1993</v>
+      </c>
+      <c r="F748" s="3" t="s">
+        <v>2208</v>
       </c>
     </row>
     <row r="750" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A750" s="3" t="s">
-        <v>2263</v>
+        <v>2209</v>
       </c>
       <c r="B750" s="3" t="s">
-        <v>2278</v>
+        <v>10</v>
+      </c>
+      <c r="C750" s="3" t="s">
+        <v>2210</v>
       </c>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A751" s="3" t="s">
-        <v>2264</v>
+        <v>2211</v>
       </c>
       <c r="B751" s="3" t="s">
-        <v>2279</v>
+        <v>28</v>
+      </c>
+      <c r="C751">
+        <v>25</v>
       </c>
     </row>
     <row r="752" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A752" s="3" t="s">
-        <v>2220</v>
+        <v>2212</v>
       </c>
       <c r="B752" s="3" t="s">
-        <v>2222</v>
+        <v>10</v>
       </c>
       <c r="C752" t="s">
-        <v>2224</v>
-      </c>
-    </row>
-    <row r="753" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A753" s="3" t="s">
-        <v>2265</v>
-      </c>
-      <c r="B753" s="3" t="s">
-        <v>2277</v>
-      </c>
-      <c r="E753" s="15" t="s">
-        <v>2266</v>
+        <v>2213</v>
+      </c>
+      <c r="F752" t="s">
+        <v>2214</v>
       </c>
     </row>
     <row r="754" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A754" s="3" t="s">
-        <v>2225</v>
+        <v>2217</v>
       </c>
       <c r="B754" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A755" s="3" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B755" s="3" t="s">
+        <v>2221</v>
+      </c>
+      <c r="C755" t="s">
+        <v>2223</v>
       </c>
     </row>
     <row r="756" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A756" s="3" t="s">
-        <v>2227</v>
+        <v>2263</v>
       </c>
       <c r="B756" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C756" t="s">
-        <v>2259</v>
-      </c>
-      <c r="E756" s="12" t="s">
-        <v>2260</v>
-      </c>
-      <c r="F756" t="s">
-        <v>2228</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="757" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A757" s="3" t="s">
-        <v>2229</v>
+        <v>2264</v>
       </c>
       <c r="B757" s="3" t="s">
-        <v>10</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="758" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A758" s="3" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B758" s="3" t="s">
+        <v>2222</v>
+      </c>
+      <c r="C758" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="759" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A759" s="3" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B759" s="3" t="s">
+        <v>2277</v>
+      </c>
+      <c r="E759" s="15" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A760" s="3" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B760" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A762" s="3" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B762" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C762" t="s">
+        <v>2259</v>
+      </c>
+      <c r="E762" s="12" t="s">
+        <v>2260</v>
+      </c>
+      <c r="F762" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A763" s="3" t="s">
+        <v>2229</v>
+      </c>
+      <c r="B763" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="764" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A764" s="3" t="s">
         <v>2231</v>
       </c>
-      <c r="B758" s="3" t="s">
+      <c r="B764" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C758" t="s">
+      <c r="C764" t="s">
         <v>1231</v>
       </c>
-      <c r="E758" t="s">
+      <c r="E764" t="s">
         <v>2232</v>
-      </c>
-    </row>
-    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A760" s="10" t="s">
-        <v>2261</v>
-      </c>
-      <c r="B760" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C760" s="13" t="s">
-        <v>2255</v>
-      </c>
-      <c r="E760" s="12" t="s">
-        <v>2267</v>
-      </c>
-      <c r="F760" s="11" t="s">
-        <v>2244</v>
-      </c>
-    </row>
-    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A761" s="10" t="s">
-        <v>2234</v>
-      </c>
-      <c r="B761" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C761" s="13" t="s">
-        <v>2256</v>
-      </c>
-      <c r="E761" s="12" t="s">
-        <v>2276</v>
-      </c>
-      <c r="F761" t="s">
-        <v>2245</v>
-      </c>
-    </row>
-    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A762" s="10" t="s">
-        <v>2235</v>
-      </c>
-      <c r="B762" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C762" s="13" t="s">
-        <v>2257</v>
-      </c>
-      <c r="E762" s="12" t="s">
-        <v>2275</v>
-      </c>
-      <c r="F762" t="s">
-        <v>2246</v>
-      </c>
-    </row>
-    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A763" s="10" t="s">
-        <v>2236</v>
-      </c>
-      <c r="B763" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C763" s="13" t="s">
-        <v>2258</v>
-      </c>
-      <c r="E763" s="12" t="s">
-        <v>2270</v>
-      </c>
-      <c r="F763" t="s">
-        <v>2247</v>
-      </c>
-    </row>
-    <row r="764" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A764" s="10" t="s">
-        <v>2237</v>
-      </c>
-      <c r="B764" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C764" s="13" t="s">
-        <v>2280</v>
-      </c>
-      <c r="E764" s="12" t="s">
-        <v>2268</v>
-      </c>
-      <c r="F764" t="s">
-        <v>2248</v>
-      </c>
-    </row>
-    <row r="765" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A765" s="10" t="s">
-        <v>2238</v>
-      </c>
-      <c r="B765" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C765" s="13" t="s">
-        <v>2281</v>
-      </c>
-      <c r="E765" s="12" t="s">
-        <v>2269</v>
-      </c>
-      <c r="F765" t="s">
-        <v>2249</v>
       </c>
     </row>
     <row r="766" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A766" s="10" t="s">
-        <v>2239</v>
+        <v>2261</v>
       </c>
       <c r="B766" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C766" s="13" t="s">
-        <v>2282</v>
+        <v>2255</v>
       </c>
       <c r="E766" s="12" t="s">
-        <v>2272</v>
-      </c>
-      <c r="F766" t="s">
-        <v>2250</v>
+        <v>2267</v>
+      </c>
+      <c r="F766" s="11" t="s">
+        <v>2244</v>
       </c>
     </row>
     <row r="767" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A767" s="10" t="s">
-        <v>2240</v>
+        <v>2234</v>
       </c>
       <c r="B767" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C767" s="13" t="s">
-        <v>2283</v>
+        <v>2256</v>
       </c>
       <c r="E767" s="12" t="s">
-        <v>2273</v>
+        <v>2276</v>
       </c>
       <c r="F767" t="s">
-        <v>2251</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="768" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A768" s="10" t="s">
-        <v>2241</v>
+        <v>2235</v>
       </c>
       <c r="B768" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C768" s="13" t="s">
-        <v>2284</v>
-      </c>
-      <c r="E768" s="12"/>
+        <v>2257</v>
+      </c>
+      <c r="E768" s="12" t="s">
+        <v>2275</v>
+      </c>
       <c r="F768" t="s">
-        <v>2252</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="769" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A769" s="10" t="s">
-        <v>2242</v>
+        <v>2236</v>
       </c>
       <c r="B769" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C769" s="13" t="s">
-        <v>2285</v>
+        <v>2258</v>
       </c>
       <c r="E769" s="12" t="s">
-        <v>2274</v>
+        <v>2270</v>
       </c>
       <c r="F769" t="s">
-        <v>2253</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="770" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A770" s="10" t="s">
-        <v>2243</v>
+        <v>2237</v>
       </c>
       <c r="B770" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C770" s="13" t="s">
+        <v>2280</v>
+      </c>
+      <c r="E770" s="12" t="s">
+        <v>2268</v>
+      </c>
+      <c r="F770" t="s">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="771" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A771" s="10" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B771" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C771" s="13" t="s">
+        <v>2281</v>
+      </c>
+      <c r="E771" s="12" t="s">
+        <v>2269</v>
+      </c>
+      <c r="F771" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A772" s="10" t="s">
+        <v>2239</v>
+      </c>
+      <c r="B772" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C772" s="13" t="s">
+        <v>2282</v>
+      </c>
+      <c r="E772" s="12" t="s">
+        <v>2272</v>
+      </c>
+      <c r="F772" t="s">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="773" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A773" s="10" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B773" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C773" s="13" t="s">
+        <v>2283</v>
+      </c>
+      <c r="E773" s="12" t="s">
+        <v>2273</v>
+      </c>
+      <c r="F773" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="774" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A774" s="10" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B774" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C774" s="13" t="s">
+        <v>2284</v>
+      </c>
+      <c r="E774" s="12"/>
+      <c r="F774" t="s">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="775" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A775" s="10" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B775" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C775" s="13" t="s">
+        <v>2285</v>
+      </c>
+      <c r="E775" s="12" t="s">
+        <v>2274</v>
+      </c>
+      <c r="F775" t="s">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="776" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A776" s="10" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B776" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C776" s="13" t="s">
         <v>2256</v>
       </c>
-      <c r="E770" s="12" t="s">
+      <c r="E776" s="12" t="s">
         <v>2271</v>
       </c>
-      <c r="F770" t="s">
+      <c r="F776" t="s">
         <v>2254</v>
       </c>
     </row>
-    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A772" s="10"/>
-      <c r="B772" s="3"/>
+    <row r="778" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A778" s="10"/>
+      <c r="B778" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -17265,8 +17336,8 @@
     <hyperlink ref="E11" r:id="rId1" display="https://w3id.org/mixs/terms/0000018" xr:uid="{E5B9998C-031F-4241-A1E7-C7E6D8677047}"/>
     <hyperlink ref="E559" r:id="rId2" xr:uid="{EC998EC6-084C-3048-AC10-E9220B7375C6}"/>
     <hyperlink ref="C730" r:id="rId3" xr:uid="{52CD8FE2-FCDC-D545-943E-8E5695A7E4C6}"/>
-    <hyperlink ref="E739" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
-    <hyperlink ref="E756" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
+    <hyperlink ref="E745" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
+    <hyperlink ref="E762" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
     <hyperlink ref="E734" r:id="rId6" xr:uid="{02045287-A2C1-2246-9C9A-09E35261DF8C}"/>
     <hyperlink ref="E733" r:id="rId7" xr:uid="{0FD7D99F-B07A-9643-9AD4-E0FEFB759009}"/>
     <hyperlink ref="E724" r:id="rId8" xr:uid="{383BC27E-9C9C-494A-88BF-6F6240C62D83}"/>
@@ -17516,10 +17587,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18106,6 +18177,48 @@
         <v>2188</v>
       </c>
       <c r="D44" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2301</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D47" t="s">
         <v>1719</v>
       </c>
     </row>
@@ -52370,10 +52483,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D255"/>
+  <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="C204" sqref="C204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54998,37 +55111,37 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B204" s="3"/>
-      <c r="C204" s="3"/>
-      <c r="D204" s="3"/>
+      <c r="A204" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>2199</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>1719</v>
+      </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>1774</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>2201</v>
+        <v>2303</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>2106</v>
-      </c>
-      <c r="D206" s="3" t="s">
-        <v>1715</v>
-      </c>
+      <c r="B206" s="3"/>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
@@ -55038,10 +55151,10 @@
         <v>2200</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>2109</v>
+        <v>2201</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -55052,7 +55165,7 @@
         <v>2200</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>1715</v>
@@ -55066,7 +55179,7 @@
         <v>2200</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>2113</v>
+        <v>2109</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>1715</v>
@@ -55080,10 +55193,10 @@
         <v>2200</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D210" s="9" t="s">
-        <v>1714</v>
+        <v>2111</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -55094,10 +55207,10 @@
         <v>2200</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="D211" s="9" t="s">
-        <v>1714</v>
+        <v>2113</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -55108,9 +55221,9 @@
         <v>2200</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="D212" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="D212" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55122,9 +55235,9 @@
         <v>2200</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>2122</v>
-      </c>
-      <c r="D213" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D213" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55136,7 +55249,7 @@
         <v>2200</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>2131</v>
+        <v>2119</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>1714</v>
@@ -55149,8 +55262,8 @@
       <c r="B215" s="3" t="s">
         <v>2200</v>
       </c>
-      <c r="C215" s="9" t="s">
-        <v>2230</v>
+      <c r="C215" s="3" t="s">
+        <v>2122</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>1714</v>
@@ -55164,7 +55277,7 @@
         <v>2200</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>1714</v>
@@ -55177,45 +55290,45 @@
       <c r="B217" s="3" t="s">
         <v>2200</v>
       </c>
-      <c r="C217" s="3" t="s">
-        <v>2136</v>
+      <c r="C217" s="9" t="s">
+        <v>2230</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B218" s="3"/>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3"/>
+      <c r="A218" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>2200</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>2134</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>1714</v>
+      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>1774</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>2201</v>
+        <v>2136</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B220" s="3" t="s">
-        <v>2202</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>2106</v>
-      </c>
-      <c r="D220" s="3" t="s">
-        <v>1715</v>
-      </c>
+      <c r="B220" s="3"/>
+      <c r="C220" s="3"/>
+      <c r="D220" s="3"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
@@ -55225,10 +55338,10 @@
         <v>2202</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>2109</v>
+        <v>2201</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -55239,7 +55352,7 @@
         <v>2202</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>1715</v>
@@ -55253,7 +55366,7 @@
         <v>2202</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>2113</v>
+        <v>2109</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>1715</v>
@@ -55267,10 +55380,10 @@
         <v>2202</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D224" s="9" t="s">
-        <v>1714</v>
+        <v>2111</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -55281,10 +55394,10 @@
         <v>2202</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="D225" s="9" t="s">
-        <v>1714</v>
+        <v>2113</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -55295,9 +55408,9 @@
         <v>2202</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="D226" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="D226" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55309,9 +55422,9 @@
         <v>2202</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>2122</v>
-      </c>
-      <c r="D227" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D227" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55323,7 +55436,7 @@
         <v>2202</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>2150</v>
+        <v>2119</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>1714</v>
@@ -55337,10 +55450,10 @@
         <v>2202</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>2152</v>
+        <v>2122</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -55351,7 +55464,7 @@
         <v>2202</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>2131</v>
+        <v>2150</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>1714</v>
@@ -55364,11 +55477,11 @@
       <c r="B231" s="3" t="s">
         <v>2202</v>
       </c>
-      <c r="C231" s="9" t="s">
-        <v>2230</v>
+      <c r="C231" s="3" t="s">
+        <v>2152</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -55379,7 +55492,7 @@
         <v>2202</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>1714</v>
@@ -55392,11 +55505,11 @@
       <c r="B233" s="3" t="s">
         <v>2202</v>
       </c>
-      <c r="C233" s="3" t="s">
-        <v>2136</v>
+      <c r="C233" s="9" t="s">
+        <v>2230</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -55407,38 +55520,38 @@
         <v>2202</v>
       </c>
       <c r="C234" s="3" t="s">
+        <v>2134</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>2202</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>2202</v>
+      </c>
+      <c r="C236" s="3" t="s">
         <v>2217</v>
       </c>
-      <c r="D234" s="3" t="s">
+      <c r="D236" s="3" t="s">
         <v>1719</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B236" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="C236" s="14" t="s">
-        <v>2104</v>
-      </c>
-      <c r="D236" s="14" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A237" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B237" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="C237" s="14" t="s">
-        <v>2106</v>
-      </c>
-      <c r="D237" s="14" t="s">
-        <v>1715</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -55449,10 +55562,10 @@
         <v>2262</v>
       </c>
       <c r="C238" s="14" t="s">
-        <v>2109</v>
+        <v>2104</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
@@ -55463,7 +55576,7 @@
         <v>2262</v>
       </c>
       <c r="C239" s="14" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
       <c r="D239" s="14" t="s">
         <v>1715</v>
@@ -55477,7 +55590,7 @@
         <v>2262</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>2113</v>
+        <v>2109</v>
       </c>
       <c r="D240" s="14" t="s">
         <v>1715</v>
@@ -55491,10 +55604,10 @@
         <v>2262</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>2115</v>
+        <v>2111</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -55505,10 +55618,10 @@
         <v>2262</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>2117</v>
+        <v>2113</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -55519,7 +55632,7 @@
         <v>2262</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>2119</v>
+        <v>2115</v>
       </c>
       <c r="D243" s="14" t="s">
         <v>1714</v>
@@ -55533,7 +55646,7 @@
         <v>2262</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>2122</v>
+        <v>2117</v>
       </c>
       <c r="D244" s="14" t="s">
         <v>1714</v>
@@ -55547,7 +55660,7 @@
         <v>2262</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>2140</v>
+        <v>2119</v>
       </c>
       <c r="D245" s="14" t="s">
         <v>1714</v>
@@ -55561,7 +55674,7 @@
         <v>2262</v>
       </c>
       <c r="C246" s="14" t="s">
-        <v>2142</v>
+        <v>2122</v>
       </c>
       <c r="D246" s="14" t="s">
         <v>1714</v>
@@ -55575,10 +55688,10 @@
         <v>2262</v>
       </c>
       <c r="C247" s="14" t="s">
-        <v>2146</v>
-      </c>
-      <c r="D247" s="9" t="s">
-        <v>1719</v>
+        <v>2140</v>
+      </c>
+      <c r="D247" s="14" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -55589,10 +55702,10 @@
         <v>2262</v>
       </c>
       <c r="C248" s="14" t="s">
-        <v>2148</v>
-      </c>
-      <c r="D248" s="9" t="s">
-        <v>1719</v>
+        <v>2142</v>
+      </c>
+      <c r="D248" s="14" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -55603,10 +55716,10 @@
         <v>2262</v>
       </c>
       <c r="C249" s="14" t="s">
-        <v>2138</v>
-      </c>
-      <c r="D249" s="14" t="s">
-        <v>1715</v>
+        <v>2146</v>
+      </c>
+      <c r="D249" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -55617,10 +55730,10 @@
         <v>2262</v>
       </c>
       <c r="C250" s="14" t="s">
-        <v>2139</v>
-      </c>
-      <c r="D250" s="14" t="s">
-        <v>1715</v>
+        <v>2148</v>
+      </c>
+      <c r="D250" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
@@ -55631,10 +55744,10 @@
         <v>2262</v>
       </c>
       <c r="C251" s="14" t="s">
-        <v>2131</v>
+        <v>2138</v>
       </c>
       <c r="D251" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
@@ -55645,10 +55758,10 @@
         <v>2262</v>
       </c>
       <c r="C252" s="14" t="s">
-        <v>2230</v>
+        <v>2139</v>
       </c>
       <c r="D252" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
@@ -55659,7 +55772,7 @@
         <v>2262</v>
       </c>
       <c r="C253" s="14" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
       <c r="D253" s="14" t="s">
         <v>1714</v>
@@ -55673,10 +55786,10 @@
         <v>2262</v>
       </c>
       <c r="C254" s="14" t="s">
-        <v>2136</v>
+        <v>2230</v>
       </c>
       <c r="D254" s="14" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
@@ -55687,9 +55800,37 @@
         <v>2262</v>
       </c>
       <c r="C255" s="14" t="s">
+        <v>2134</v>
+      </c>
+      <c r="D255" s="14" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B256" s="14" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C256" s="14" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D256" s="14" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B257" s="14" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C257" s="14" t="s">
         <v>2217</v>
       </c>
-      <c r="D255" s="14" t="s">
+      <c r="D257" s="14" t="s">
         <v>1719</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated sample concentration and sample concentration unit to take unknown values
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdaws/Documents/FAIRDS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdaws/Documents/fairds_storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9064C0B-8CD0-864F-B586-EEB5B2D1CB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF39E4B-4721-3543-9034-E5009C63AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regex" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13642" uniqueCount="2305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13612" uniqueCount="2301">
   <si>
     <t>short hand form</t>
   </si>
@@ -6395,9 +6395,6 @@
   </si>
   <si>
     <t>sample concentration unit</t>
-  </si>
-  <si>
-    <t>{text}{1,3}/{text}{1,3}</t>
   </si>
   <si>
     <t>ug/mL</t>
@@ -7096,19 +7093,10 @@
     <t>http://purl.obolibrary.org/obo/MS_1000465</t>
   </si>
   <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>additional data processing protocol</t>
-  </si>
-  <si>
-    <t>labnotes as pdf</t>
-  </si>
-  <si>
-    <t>fitzpatrick</t>
+    <t>({float}|unknown)</t>
+  </si>
+  <si>
+    <t>({text}{1,3}/{text}{1,3}|unknown)</t>
   </si>
 </sst>
 </file>
@@ -7921,11 +7909,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F778"/>
+  <dimension ref="A1:F772"/>
   <sheetViews>
-    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A737" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B739" sqref="B739"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A685" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B689" sqref="B689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16350,7 +16338,7 @@
         <v>60</v>
       </c>
       <c r="C698" s="8" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="F698" s="3" t="s">
         <v>2114</v>
@@ -16389,7 +16377,7 @@
         <v>2119</v>
       </c>
       <c r="B701" s="3" t="s">
-        <v>55</v>
+        <v>2299</v>
       </c>
       <c r="C701" s="3" t="s">
         <v>2120</v>
@@ -16403,60 +16391,60 @@
         <v>2122</v>
       </c>
       <c r="B702" s="3" t="s">
+        <v>2300</v>
+      </c>
+      <c r="C702" s="3" t="s">
         <v>2123</v>
       </c>
-      <c r="C702" s="3" t="s">
+      <c r="F702" s="3" t="s">
         <v>2124</v>
-      </c>
-      <c r="F702" s="3" t="s">
-        <v>2125</v>
       </c>
     </row>
     <row r="703" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A703" s="3" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="B703" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C703" s="3" t="s">
+        <v>2126</v>
+      </c>
+      <c r="F703" s="3" t="s">
         <v>2127</v>
-      </c>
-      <c r="F703" s="3" t="s">
-        <v>2128</v>
       </c>
     </row>
     <row r="704" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A704" s="3" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="B704" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C704" s="3" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="F704" s="3" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="705" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A705" s="3" t="s">
+        <v>2130</v>
+      </c>
+      <c r="B705" s="3" t="s">
+        <v>2285</v>
+      </c>
+      <c r="C705" s="6" t="s">
+        <v>2203</v>
+      </c>
+      <c r="F705" s="3" t="s">
         <v>2131</v>
-      </c>
-      <c r="B705" s="3" t="s">
-        <v>2286</v>
-      </c>
-      <c r="C705" s="6" t="s">
-        <v>2204</v>
-      </c>
-      <c r="F705" s="3" t="s">
-        <v>2132</v>
       </c>
     </row>
     <row r="706" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A706" s="3" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="B706" s="3" t="s">
         <v>78</v>
@@ -16465,68 +16453,68 @@
         <v>1</v>
       </c>
       <c r="F706" s="3" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="707" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A707" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="B707" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C707" s="6" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="F707" s="3" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="708" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A708" s="3" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="B708" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C708" s="6" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="F708" s="3" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="710" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A710" s="3" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="B710" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C710" s="3" t="s">
+        <v>2126</v>
+      </c>
+      <c r="F710" s="3" t="s">
         <v>2127</v>
-      </c>
-      <c r="F710" s="3" t="s">
-        <v>2128</v>
       </c>
     </row>
     <row r="711" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A711" s="3" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="B711" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C711" s="3" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="F711" s="3" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="712" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A712" s="3" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="B712" s="3" t="s">
         <v>55</v>
@@ -16535,26 +16523,26 @@
         <v>195</v>
       </c>
       <c r="F712" s="3" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="713" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A713" s="3" t="s">
+        <v>2141</v>
+      </c>
+      <c r="B713" s="3" t="s">
         <v>2142</v>
       </c>
-      <c r="B713" s="3" t="s">
+      <c r="C713" s="3" t="s">
         <v>2143</v>
       </c>
-      <c r="C713" s="3" t="s">
+      <c r="F713" s="3" t="s">
         <v>2144</v>
-      </c>
-      <c r="F713" s="3" t="s">
-        <v>2145</v>
       </c>
     </row>
     <row r="714" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A714" s="3" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B714" s="3" t="s">
         <v>55</v>
@@ -16563,26 +16551,26 @@
         <v>58695</v>
       </c>
       <c r="F714" s="3" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="715" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A715" s="3" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B715" s="3" t="s">
+        <v>2142</v>
+      </c>
+      <c r="C715" s="3" t="s">
+        <v>2143</v>
+      </c>
+      <c r="F715" s="3" t="s">
         <v>2148</v>
-      </c>
-      <c r="B715" s="3" t="s">
-        <v>2143</v>
-      </c>
-      <c r="C715" s="3" t="s">
-        <v>2144</v>
-      </c>
-      <c r="F715" s="3" t="s">
-        <v>2149</v>
       </c>
     </row>
     <row r="716" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A716" s="3" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="B716" s="3" t="s">
         <v>55</v>
@@ -16593,7 +16581,7 @@
     </row>
     <row r="718" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A718" s="3" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="B718" s="3" t="s">
         <v>10</v>
@@ -16602,12 +16590,12 @@
         <v>74</v>
       </c>
       <c r="F718" s="3" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="719" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A719" s="3" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="B719" s="3" t="s">
         <v>10</v>
@@ -16616,7 +16604,7 @@
         <v>74</v>
       </c>
       <c r="F719" s="3" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="720" spans="1:6" x14ac:dyDescent="0.2">
@@ -16627,64 +16615,64 @@
     </row>
     <row r="721" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A721" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="B721" s="3" t="s">
         <v>241</v>
       </c>
       <c r="C721" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="722" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A722" s="3" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="B722" s="3" t="s">
         <v>241</v>
       </c>
       <c r="C722" s="3" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="E722" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F722" s="3" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="723" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A723" s="3" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B723" s="3" t="s">
         <v>2157</v>
       </c>
-      <c r="B723" s="3" t="s">
+      <c r="C723" s="3" t="s">
         <v>2158</v>
-      </c>
-      <c r="C723" s="3" t="s">
-        <v>2159</v>
       </c>
       <c r="E723" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F723" s="3" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="724" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A724" s="3" t="s">
+        <v>2295</v>
+      </c>
+      <c r="B724" s="3" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C724" s="3" t="s">
+        <v>2223</v>
+      </c>
+      <c r="E724" s="2" t="s">
+        <v>2298</v>
+      </c>
+      <c r="F724" s="3" t="s">
         <v>2296</v>
-      </c>
-      <c r="B724" s="3" t="s">
-        <v>2298</v>
-      </c>
-      <c r="C724" s="3" t="s">
-        <v>2224</v>
-      </c>
-      <c r="E724" s="2" t="s">
-        <v>2299</v>
-      </c>
-      <c r="F724" s="3" t="s">
-        <v>2297</v>
       </c>
     </row>
     <row r="725" spans="1:6" x14ac:dyDescent="0.2">
@@ -16696,7 +16684,7 @@
     </row>
     <row r="726" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A726" s="3" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="B726" s="3" t="s">
         <v>28</v>
@@ -16709,24 +16697,24 @@
     </row>
     <row r="727" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A727" s="3" t="s">
+        <v>2161</v>
+      </c>
+      <c r="B727" s="3" t="s">
+        <v>2157</v>
+      </c>
+      <c r="C727" s="3" t="s">
         <v>2162</v>
-      </c>
-      <c r="B727" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="C727" s="3" t="s">
-        <v>2163</v>
       </c>
       <c r="E727" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F727" s="3" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="728" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A728" s="3" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="B728" s="3" t="s">
         <v>28</v>
@@ -16739,56 +16727,56 @@
     </row>
     <row r="729" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A729" s="3" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B729" s="3" t="s">
         <v>2166</v>
       </c>
-      <c r="B729" s="3" t="s">
+      <c r="C729" s="3" t="s">
         <v>2167</v>
-      </c>
-      <c r="C729" s="3" t="s">
-        <v>2168</v>
       </c>
       <c r="E729" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F729" s="3" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="730" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A730" s="3" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B730" s="3" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="C730" s="2" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="E730" s="3"/>
       <c r="F730" s="3" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="731" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A731" s="3" t="s">
+        <v>2171</v>
+      </c>
+      <c r="B731" s="3" t="s">
+        <v>2166</v>
+      </c>
+      <c r="C731" s="3" t="s">
         <v>2172</v>
-      </c>
-      <c r="B731" s="3" t="s">
-        <v>2167</v>
-      </c>
-      <c r="C731" s="3" t="s">
-        <v>2173</v>
       </c>
       <c r="E731" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F731" s="3" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="732" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A732" s="3" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="B732" s="3" t="s">
         <v>67</v>
@@ -16800,535 +16788,479 @@
         <v>388</v>
       </c>
       <c r="F732" s="3" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="733" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A733" s="3" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="B733" s="3" t="s">
         <v>241</v>
       </c>
       <c r="C733" s="3" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="E733" s="2" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="F733" s="3"/>
     </row>
     <row r="734" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A734" s="3" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="B734" s="3" t="s">
         <v>241</v>
       </c>
       <c r="C734" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="E734" s="2" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="F734" s="3" t="s">
-        <v>2291</v>
-      </c>
-    </row>
-    <row r="735" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A735" s="3" t="s">
-        <v>2300</v>
-      </c>
-      <c r="B735" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E735" s="2"/>
-      <c r="F735" s="3"/>
+        <v>2290</v>
+      </c>
     </row>
     <row r="736" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A736" s="3" t="s">
-        <v>2301</v>
+        <v>2176</v>
       </c>
       <c r="B736" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E736" s="2"/>
-      <c r="F736" s="3"/>
+        <v>2157</v>
+      </c>
+      <c r="C736" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E736" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F736" s="3" t="s">
+        <v>2176</v>
+      </c>
     </row>
     <row r="737" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A737" s="3" t="s">
-        <v>2304</v>
+        <v>2177</v>
       </c>
       <c r="B737" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E737" s="2"/>
-      <c r="F737" s="3"/>
+        <v>2157</v>
+      </c>
+      <c r="C737" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E737" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F737" s="3" t="s">
+        <v>2178</v>
+      </c>
     </row>
     <row r="738" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A738" s="3" t="s">
-        <v>2302</v>
+        <v>2206</v>
       </c>
       <c r="B738" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E738" s="2"/>
-      <c r="F738" s="3"/>
+        <v>2179</v>
+      </c>
+      <c r="C738" s="3" t="s">
+        <v>2180</v>
+      </c>
+      <c r="E738" s="3"/>
+      <c r="F738" s="3" t="s">
+        <v>2181</v>
+      </c>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A739" s="3" t="s">
-        <v>2303</v>
+        <v>2182</v>
       </c>
       <c r="B739" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="C739" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E739" s="2" t="s">
+        <v>2205</v>
+      </c>
+      <c r="F739" s="3" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="740" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A740" s="3" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B740" s="3" t="s">
+        <v>2215</v>
+      </c>
+      <c r="C740" s="3" t="s">
+        <v>2185</v>
+      </c>
+      <c r="E740" s="3"/>
+      <c r="F740" s="3" t="s">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="741" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A741" s="3" t="s">
+        <v>2187</v>
+      </c>
+      <c r="B741" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E739" s="2"/>
-      <c r="F739" s="3"/>
-    </row>
-    <row r="740" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A740" s="3"/>
-      <c r="B740" s="3"/>
-      <c r="E740" s="2"/>
-      <c r="F740" s="3"/>
+      <c r="C741" s="3" t="s">
+        <v>2188</v>
+      </c>
+      <c r="E741" s="3"/>
+      <c r="F741" s="3" t="s">
+        <v>2189</v>
+      </c>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A742" s="3" t="s">
-        <v>2177</v>
+        <v>2207</v>
       </c>
       <c r="B742" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="C742" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E742" s="3" t="s">
-        <v>194</v>
+        <v>2214</v>
+      </c>
+      <c r="C742">
+        <v>1993</v>
       </c>
       <c r="F742" s="3" t="s">
-        <v>2177</v>
-      </c>
-    </row>
-    <row r="743" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A743" s="3" t="s">
-        <v>2178</v>
-      </c>
-      <c r="B743" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="C743" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E743" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F743" s="3" t="s">
-        <v>2179</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A744" s="3" t="s">
-        <v>2207</v>
+        <v>2208</v>
       </c>
       <c r="B744" s="3" t="s">
-        <v>2180</v>
+        <v>10</v>
       </c>
       <c r="C744" s="3" t="s">
-        <v>2181</v>
-      </c>
-      <c r="E744" s="3"/>
-      <c r="F744" s="3" t="s">
-        <v>2182</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A745" s="3" t="s">
-        <v>2183</v>
+        <v>2210</v>
       </c>
       <c r="B745" s="3" t="s">
-        <v>847</v>
-      </c>
-      <c r="C745" s="3" t="s">
-        <v>1408</v>
-      </c>
-      <c r="E745" s="2" t="s">
-        <v>2206</v>
-      </c>
-      <c r="F745" s="3" t="s">
-        <v>2184</v>
+        <v>28</v>
+      </c>
+      <c r="C745">
+        <v>25</v>
       </c>
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A746" s="3" t="s">
-        <v>2185</v>
+        <v>2211</v>
       </c>
       <c r="B746" s="3" t="s">
-        <v>2216</v>
-      </c>
-      <c r="C746" s="3" t="s">
-        <v>2186</v>
-      </c>
-      <c r="E746" s="3"/>
-      <c r="F746" s="3" t="s">
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="747" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A747" s="3" t="s">
-        <v>2188</v>
-      </c>
-      <c r="B747" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C747" s="3" t="s">
-        <v>2189</v>
-      </c>
-      <c r="E747" s="3"/>
-      <c r="F747" s="3" t="s">
-        <v>2190</v>
+        <v>10</v>
+      </c>
+      <c r="C746" t="s">
+        <v>2212</v>
+      </c>
+      <c r="F746" t="s">
+        <v>2213</v>
       </c>
     </row>
     <row r="748" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A748" s="3" t="s">
-        <v>2208</v>
+        <v>2216</v>
       </c>
       <c r="B748" s="3" t="s">
-        <v>2215</v>
-      </c>
-      <c r="C748">
-        <v>1993</v>
-      </c>
-      <c r="F748" s="3" t="s">
-        <v>2208</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="749" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A749" s="3" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B749" s="3" t="s">
+        <v>2220</v>
+      </c>
+      <c r="C749" t="s">
+        <v>2222</v>
       </c>
     </row>
     <row r="750" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A750" s="3" t="s">
-        <v>2209</v>
+        <v>2262</v>
       </c>
       <c r="B750" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C750" s="3" t="s">
-        <v>2210</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A751" s="3" t="s">
-        <v>2211</v>
+        <v>2263</v>
       </c>
       <c r="B751" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C751">
-        <v>25</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="752" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A752" s="3" t="s">
-        <v>2212</v>
+        <v>2219</v>
       </c>
       <c r="B752" s="3" t="s">
-        <v>10</v>
+        <v>2221</v>
       </c>
       <c r="C752" t="s">
-        <v>2213</v>
-      </c>
-      <c r="F752" t="s">
-        <v>2214</v>
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A753" s="3" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B753" s="3" t="s">
+        <v>2276</v>
+      </c>
+      <c r="E753" s="15" t="s">
+        <v>2265</v>
       </c>
     </row>
     <row r="754" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A754" s="3" t="s">
-        <v>2217</v>
+        <v>2224</v>
       </c>
       <c r="B754" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A755" s="3" t="s">
-        <v>2219</v>
-      </c>
-      <c r="B755" s="3" t="s">
-        <v>2221</v>
-      </c>
-      <c r="C755" t="s">
-        <v>2223</v>
+        <v>50</v>
       </c>
     </row>
     <row r="756" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A756" s="3" t="s">
-        <v>2263</v>
+        <v>2226</v>
       </c>
       <c r="B756" s="3" t="s">
-        <v>2278</v>
+        <v>10</v>
+      </c>
+      <c r="C756" t="s">
+        <v>2258</v>
+      </c>
+      <c r="E756" s="12" t="s">
+        <v>2259</v>
+      </c>
+      <c r="F756" t="s">
+        <v>2227</v>
       </c>
     </row>
     <row r="757" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A757" s="3" t="s">
-        <v>2264</v>
+        <v>2228</v>
       </c>
       <c r="B757" s="3" t="s">
-        <v>2279</v>
+        <v>10</v>
       </c>
     </row>
     <row r="758" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A758" s="3" t="s">
-        <v>2220</v>
+        <v>2230</v>
       </c>
       <c r="B758" s="3" t="s">
-        <v>2222</v>
+        <v>98</v>
       </c>
       <c r="C758" t="s">
-        <v>2224</v>
-      </c>
-    </row>
-    <row r="759" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A759" s="3" t="s">
-        <v>2265</v>
-      </c>
-      <c r="B759" s="3" t="s">
-        <v>2277</v>
-      </c>
-      <c r="E759" s="15" t="s">
+        <v>1231</v>
+      </c>
+      <c r="E758" t="s">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A760" s="10" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B760" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C760" s="13" t="s">
+        <v>2254</v>
+      </c>
+      <c r="E760" s="12" t="s">
         <v>2266</v>
       </c>
-    </row>
-    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A760" s="3" t="s">
-        <v>2225</v>
-      </c>
-      <c r="B760" s="3" t="s">
-        <v>50</v>
+      <c r="F760" s="11" t="s">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A761" s="10" t="s">
+        <v>2233</v>
+      </c>
+      <c r="B761" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C761" s="13" t="s">
+        <v>2255</v>
+      </c>
+      <c r="E761" s="12" t="s">
+        <v>2275</v>
+      </c>
+      <c r="F761" t="s">
+        <v>2244</v>
       </c>
     </row>
     <row r="762" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A762" s="3" t="s">
-        <v>2227</v>
+      <c r="A762" s="10" t="s">
+        <v>2234</v>
       </c>
       <c r="B762" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C762" t="s">
-        <v>2259</v>
+        <v>55</v>
+      </c>
+      <c r="C762" s="13" t="s">
+        <v>2256</v>
       </c>
       <c r="E762" s="12" t="s">
-        <v>2260</v>
+        <v>2274</v>
       </c>
       <c r="F762" t="s">
-        <v>2228</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="763" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A763" s="3" t="s">
-        <v>2229</v>
+      <c r="A763" s="10" t="s">
+        <v>2235</v>
       </c>
       <c r="B763" s="3" t="s">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="C763" s="13" t="s">
+        <v>2257</v>
+      </c>
+      <c r="E763" s="12" t="s">
+        <v>2269</v>
+      </c>
+      <c r="F763" t="s">
+        <v>2246</v>
       </c>
     </row>
     <row r="764" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A764" s="3" t="s">
-        <v>2231</v>
+      <c r="A764" s="10" t="s">
+        <v>2236</v>
       </c>
       <c r="B764" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C764" t="s">
-        <v>1231</v>
-      </c>
-      <c r="E764" t="s">
-        <v>2232</v>
+        <v>55</v>
+      </c>
+      <c r="C764" s="13" t="s">
+        <v>2279</v>
+      </c>
+      <c r="E764" s="12" t="s">
+        <v>2267</v>
+      </c>
+      <c r="F764" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="765" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A765" s="10" t="s">
+        <v>2237</v>
+      </c>
+      <c r="B765" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C765" s="13" t="s">
+        <v>2280</v>
+      </c>
+      <c r="E765" s="12" t="s">
+        <v>2268</v>
+      </c>
+      <c r="F765" t="s">
+        <v>2248</v>
       </c>
     </row>
     <row r="766" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A766" s="10" t="s">
-        <v>2261</v>
+        <v>2238</v>
       </c>
       <c r="B766" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C766" s="13" t="s">
-        <v>2255</v>
+        <v>2281</v>
       </c>
       <c r="E766" s="12" t="s">
-        <v>2267</v>
-      </c>
-      <c r="F766" s="11" t="s">
-        <v>2244</v>
+        <v>2271</v>
+      </c>
+      <c r="F766" t="s">
+        <v>2249</v>
       </c>
     </row>
     <row r="767" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A767" s="10" t="s">
-        <v>2234</v>
+        <v>2239</v>
       </c>
       <c r="B767" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C767" s="13" t="s">
-        <v>2256</v>
+        <v>2282</v>
       </c>
       <c r="E767" s="12" t="s">
-        <v>2276</v>
+        <v>2272</v>
       </c>
       <c r="F767" t="s">
-        <v>2245</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="768" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A768" s="10" t="s">
-        <v>2235</v>
+        <v>2240</v>
       </c>
       <c r="B768" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C768" s="13" t="s">
-        <v>2257</v>
-      </c>
-      <c r="E768" s="12" t="s">
-        <v>2275</v>
-      </c>
+        <v>2283</v>
+      </c>
+      <c r="E768" s="12"/>
       <c r="F768" t="s">
-        <v>2246</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="769" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A769" s="10" t="s">
-        <v>2236</v>
+        <v>2241</v>
       </c>
       <c r="B769" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C769" s="13" t="s">
-        <v>2258</v>
+        <v>2284</v>
       </c>
       <c r="E769" s="12" t="s">
-        <v>2270</v>
+        <v>2273</v>
       </c>
       <c r="F769" t="s">
-        <v>2247</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="770" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A770" s="10" t="s">
-        <v>2237</v>
+        <v>2242</v>
       </c>
       <c r="B770" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C770" s="13" t="s">
-        <v>2280</v>
+        <v>2255</v>
       </c>
       <c r="E770" s="12" t="s">
-        <v>2268</v>
+        <v>2270</v>
       </c>
       <c r="F770" t="s">
-        <v>2248</v>
-      </c>
-    </row>
-    <row r="771" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A771" s="10" t="s">
-        <v>2238</v>
-      </c>
-      <c r="B771" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C771" s="13" t="s">
-        <v>2281</v>
-      </c>
-      <c r="E771" s="12" t="s">
-        <v>2269</v>
-      </c>
-      <c r="F771" t="s">
-        <v>2249</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="772" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A772" s="10" t="s">
-        <v>2239</v>
-      </c>
-      <c r="B772" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C772" s="13" t="s">
-        <v>2282</v>
-      </c>
-      <c r="E772" s="12" t="s">
-        <v>2272</v>
-      </c>
-      <c r="F772" t="s">
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="773" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A773" s="10" t="s">
-        <v>2240</v>
-      </c>
-      <c r="B773" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C773" s="13" t="s">
-        <v>2283</v>
-      </c>
-      <c r="E773" s="12" t="s">
-        <v>2273</v>
-      </c>
-      <c r="F773" t="s">
-        <v>2251</v>
-      </c>
-    </row>
-    <row r="774" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A774" s="10" t="s">
-        <v>2241</v>
-      </c>
-      <c r="B774" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C774" s="13" t="s">
-        <v>2284</v>
-      </c>
-      <c r="E774" s="12"/>
-      <c r="F774" t="s">
-        <v>2252</v>
-      </c>
-    </row>
-    <row r="775" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A775" s="10" t="s">
-        <v>2242</v>
-      </c>
-      <c r="B775" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C775" s="13" t="s">
-        <v>2285</v>
-      </c>
-      <c r="E775" s="12" t="s">
-        <v>2274</v>
-      </c>
-      <c r="F775" t="s">
-        <v>2253</v>
-      </c>
-    </row>
-    <row r="776" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A776" s="10" t="s">
-        <v>2243</v>
-      </c>
-      <c r="B776" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C776" s="13" t="s">
-        <v>2256</v>
-      </c>
-      <c r="E776" s="12" t="s">
-        <v>2271</v>
-      </c>
-      <c r="F776" t="s">
-        <v>2254</v>
-      </c>
-    </row>
-    <row r="778" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A778" s="10"/>
-      <c r="B778" s="3"/>
+      <c r="A772" s="10"/>
+      <c r="B772" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -17336,8 +17268,8 @@
     <hyperlink ref="E11" r:id="rId1" display="https://w3id.org/mixs/terms/0000018" xr:uid="{E5B9998C-031F-4241-A1E7-C7E6D8677047}"/>
     <hyperlink ref="E559" r:id="rId2" xr:uid="{EC998EC6-084C-3048-AC10-E9220B7375C6}"/>
     <hyperlink ref="C730" r:id="rId3" xr:uid="{52CD8FE2-FCDC-D545-943E-8E5695A7E4C6}"/>
-    <hyperlink ref="E745" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
-    <hyperlink ref="E762" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
+    <hyperlink ref="E739" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
+    <hyperlink ref="E756" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
     <hyperlink ref="E734" r:id="rId6" xr:uid="{02045287-A2C1-2246-9C9A-09E35261DF8C}"/>
     <hyperlink ref="E733" r:id="rId7" xr:uid="{0FD7D99F-B07A-9643-9AD4-E0FEFB759009}"/>
     <hyperlink ref="E724" r:id="rId8" xr:uid="{383BC27E-9C9C-494A-88BF-6F6240C62D83}"/>
@@ -17587,10 +17519,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17749,7 +17681,7 @@
         <v>1718</v>
       </c>
       <c r="C12" t="s">
-        <v>2265</v>
+        <v>2264</v>
       </c>
       <c r="D12" t="s">
         <v>1719</v>
@@ -17763,7 +17695,7 @@
         <v>1718</v>
       </c>
       <c r="C13" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="D13" t="s">
         <v>1719</v>
@@ -17777,7 +17709,7 @@
         <v>1718</v>
       </c>
       <c r="C14" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="D14" t="s">
         <v>1719</v>
@@ -17791,7 +17723,7 @@
         <v>1718</v>
       </c>
       <c r="C15" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="D15" t="s">
         <v>1719</v>
@@ -17805,7 +17737,7 @@
         <v>1718</v>
       </c>
       <c r="C16" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
       <c r="D16" t="s">
         <v>1719</v>
@@ -17833,7 +17765,7 @@
         <v>1718</v>
       </c>
       <c r="C18" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="D18" t="s">
         <v>1719</v>
@@ -17861,13 +17793,13 @@
         <v>1718</v>
       </c>
       <c r="C20" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="D20" t="s">
         <v>1715</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -17878,13 +17810,13 @@
         <v>1718</v>
       </c>
       <c r="C21" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
       <c r="D21" t="s">
         <v>1715</v>
       </c>
       <c r="G21" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -17895,13 +17827,13 @@
         <v>1718</v>
       </c>
       <c r="C22" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="D22" t="s">
         <v>1715</v>
       </c>
       <c r="G22" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -17912,13 +17844,13 @@
         <v>1718</v>
       </c>
       <c r="C23" t="s">
-        <v>2236</v>
+        <v>2235</v>
       </c>
       <c r="D23" t="s">
         <v>1715</v>
       </c>
       <c r="G23" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -17929,13 +17861,13 @@
         <v>1718</v>
       </c>
       <c r="C24" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="D24" t="s">
         <v>1715</v>
       </c>
       <c r="G24" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -17946,13 +17878,13 @@
         <v>1718</v>
       </c>
       <c r="C25" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="D25" t="s">
         <v>1715</v>
       </c>
       <c r="G25" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -17963,13 +17895,13 @@
         <v>1718</v>
       </c>
       <c r="C26" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="D26" t="s">
         <v>1715</v>
       </c>
       <c r="G26" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -17980,13 +17912,13 @@
         <v>1718</v>
       </c>
       <c r="C27" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="D27" t="s">
         <v>1715</v>
       </c>
       <c r="G27" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -17997,13 +17929,13 @@
         <v>1718</v>
       </c>
       <c r="C28" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="D28" t="s">
         <v>1715</v>
       </c>
       <c r="G28" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -18014,13 +17946,13 @@
         <v>1718</v>
       </c>
       <c r="C29" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="D29" t="s">
         <v>1715</v>
       </c>
       <c r="G29" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -18031,13 +17963,13 @@
         <v>1718</v>
       </c>
       <c r="C30" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="D30" t="s">
         <v>1715</v>
       </c>
       <c r="G30" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -18045,10 +17977,10 @@
         <v>1717</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="D35" t="s">
         <v>1719</v>
@@ -18059,10 +17991,10 @@
         <v>1717</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="D36" t="s">
         <v>1719</v>
@@ -18073,10 +18005,10 @@
         <v>1717</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="D37" t="s">
         <v>1719</v>
@@ -18087,10 +18019,10 @@
         <v>1717</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="D38" t="s">
         <v>1714</v>
@@ -18101,7 +18033,7 @@
         <v>1717</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>1162</v>
@@ -18115,10 +18047,10 @@
         <v>1717</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="D40" t="s">
         <v>1714</v>
@@ -18129,7 +18061,7 @@
         <v>1717</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>675</v>
@@ -18143,10 +18075,10 @@
         <v>1717</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="D42" t="s">
         <v>1719</v>
@@ -18157,7 +18089,7 @@
         <v>1717</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>1152</v>
@@ -18171,54 +18103,12 @@
         <v>1717</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="D44" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>2191</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>2300</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>2191</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>2301</v>
-      </c>
-      <c r="D46" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B47" t="s">
-        <v>2191</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>2304</v>
-      </c>
-      <c r="D47" t="s">
         <v>1719</v>
       </c>
     </row>
@@ -18232,7 +18122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2459"/>
   <sheetViews>
-    <sheetView topLeftCell="A2413" workbookViewId="0">
+    <sheetView topLeftCell="A2412" workbookViewId="0">
       <selection activeCell="C2456" sqref="C2456"/>
     </sheetView>
   </sheetViews>
@@ -52157,10 +52047,10 @@
         <v>1720</v>
       </c>
       <c r="B2426" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2426" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="D2426" t="s">
         <v>1719</v>
@@ -52171,10 +52061,10 @@
         <v>1720</v>
       </c>
       <c r="B2427" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2427" s="3" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="D2427" t="s">
         <v>1719</v>
@@ -52185,10 +52075,10 @@
         <v>1720</v>
       </c>
       <c r="B2428" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2428" s="3" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="D2428" t="s">
         <v>1714</v>
@@ -52199,10 +52089,10 @@
         <v>1720</v>
       </c>
       <c r="B2429" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2429" s="3" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="D2429" t="s">
         <v>1715</v>
@@ -52213,10 +52103,10 @@
         <v>1720</v>
       </c>
       <c r="B2430" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2430" s="3" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="D2430" t="s">
         <v>1714</v>
@@ -52227,10 +52117,10 @@
         <v>1720</v>
       </c>
       <c r="B2431" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2431" s="3" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D2431" t="s">
         <v>1715</v>
@@ -52241,10 +52131,10 @@
         <v>1720</v>
       </c>
       <c r="B2432" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2432" s="3" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="D2432" t="s">
         <v>1714</v>
@@ -52255,7 +52145,7 @@
         <v>1720</v>
       </c>
       <c r="B2433" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2433" s="3" t="s">
         <v>1557</v>
@@ -52269,10 +52159,10 @@
         <v>1720</v>
       </c>
       <c r="B2434" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2434" s="3" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="D2434" t="s">
         <v>1719</v>
@@ -52283,10 +52173,10 @@
         <v>1720</v>
       </c>
       <c r="B2435" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2435" s="3" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="D2435" t="s">
         <v>1719</v>
@@ -52297,10 +52187,10 @@
         <v>1720</v>
       </c>
       <c r="B2436" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2436" s="3" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="D2436" t="s">
         <v>1719</v>
@@ -52311,10 +52201,10 @@
         <v>1720</v>
       </c>
       <c r="B2437" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2437" s="3" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="D2437" t="s">
         <v>1719</v>
@@ -52325,10 +52215,10 @@
         <v>1720</v>
       </c>
       <c r="B2438" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2438" s="3" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="D2438" t="s">
         <v>1714</v>
@@ -52339,10 +52229,10 @@
         <v>1720</v>
       </c>
       <c r="B2439" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2439" s="3" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="D2439" t="s">
         <v>1714</v>
@@ -52353,7 +52243,7 @@
         <v>1720</v>
       </c>
       <c r="B2440" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2440" s="3" t="s">
         <v>1152</v>
@@ -52367,10 +52257,10 @@
         <v>1720</v>
       </c>
       <c r="B2441" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2441" s="16" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="D2441" t="s">
         <v>1719</v>
@@ -52381,10 +52271,10 @@
         <v>1720</v>
       </c>
       <c r="B2442" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="C2442" s="3" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="D2442" t="s">
         <v>1719</v>
@@ -52399,10 +52289,10 @@
         <v>1720</v>
       </c>
       <c r="B2444" s="3" t="s">
+        <v>2225</v>
+      </c>
+      <c r="C2444" s="3" t="s">
         <v>2226</v>
-      </c>
-      <c r="C2444" s="3" t="s">
-        <v>2227</v>
       </c>
       <c r="D2444" t="s">
         <v>1715</v>
@@ -52413,10 +52303,10 @@
         <v>1720</v>
       </c>
       <c r="B2445" s="3" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="C2445" s="3" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="D2445" t="s">
         <v>1715</v>
@@ -52427,10 +52317,10 @@
         <v>1720</v>
       </c>
       <c r="B2446" s="3" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="C2446" s="3" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D2446" t="s">
         <v>1715</v>
@@ -52483,10 +52373,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D257"/>
+  <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="C204" sqref="C204"/>
+    <sheetView topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53592,7 +53482,7 @@
         <v>1774</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>2104</v>
@@ -53606,7 +53496,7 @@
         <v>1774</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>2106</v>
@@ -53620,7 +53510,7 @@
         <v>1774</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>2109</v>
@@ -53634,7 +53524,7 @@
         <v>1774</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>2111</v>
@@ -53648,7 +53538,7 @@
         <v>1774</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>2113</v>
@@ -53662,7 +53552,7 @@
         <v>1774</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>2115</v>
@@ -53676,7 +53566,7 @@
         <v>1774</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>2117</v>
@@ -53690,7 +53580,7 @@
         <v>1774</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>2119</v>
@@ -53704,7 +53594,7 @@
         <v>1774</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>2122</v>
@@ -53718,10 +53608,10 @@
         <v>1774</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>1715</v>
@@ -53732,10 +53622,10 @@
         <v>1774</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>1715</v>
@@ -53746,10 +53636,10 @@
         <v>1774</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>1714</v>
@@ -53760,10 +53650,10 @@
         <v>1774</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>1714</v>
@@ -53774,10 +53664,10 @@
         <v>1774</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>1714</v>
@@ -53788,10 +53678,10 @@
         <v>1774</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>1719</v>
@@ -53802,10 +53692,10 @@
         <v>1774</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>1719</v>
@@ -53816,10 +53706,10 @@
         <v>1774</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>1719</v>
@@ -53830,10 +53720,10 @@
         <v>1774</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>1714</v>
@@ -53844,10 +53734,10 @@
         <v>1774</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>1714</v>
@@ -53858,10 +53748,10 @@
         <v>1774</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>1719</v>
@@ -53877,7 +53767,7 @@
         <v>1774</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>2104</v>
@@ -53891,7 +53781,7 @@
         <v>1774</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>2106</v>
@@ -53905,7 +53795,7 @@
         <v>1774</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>2119</v>
@@ -53919,7 +53809,7 @@
         <v>1774</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>2122</v>
@@ -53933,10 +53823,10 @@
         <v>1774</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>1715</v>
@@ -53947,10 +53837,10 @@
         <v>1774</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>1715</v>
@@ -53961,10 +53851,10 @@
         <v>1774</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>1714</v>
@@ -53975,10 +53865,10 @@
         <v>1774</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>1714</v>
@@ -53989,10 +53879,10 @@
         <v>1774</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>1714</v>
@@ -54003,10 +53893,10 @@
         <v>1774</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>1719</v>
@@ -54017,10 +53907,10 @@
         <v>1774</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>1719</v>
@@ -54031,10 +53921,10 @@
         <v>1774</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>1719</v>
@@ -54045,10 +53935,10 @@
         <v>1774</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>1714</v>
@@ -54059,10 +53949,10 @@
         <v>1774</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>1714</v>
@@ -54073,10 +53963,10 @@
         <v>1774</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>1719</v>
@@ -54092,7 +53982,7 @@
         <v>1774</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>2104</v>
@@ -54106,7 +53996,7 @@
         <v>1774</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>2106</v>
@@ -54120,7 +54010,7 @@
         <v>1774</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>2109</v>
@@ -54134,7 +54024,7 @@
         <v>1774</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>2111</v>
@@ -54148,7 +54038,7 @@
         <v>1774</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>2113</v>
@@ -54162,7 +54052,7 @@
         <v>1774</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>2115</v>
@@ -54176,7 +54066,7 @@
         <v>1774</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>2117</v>
@@ -54190,7 +54080,7 @@
         <v>1774</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>2119</v>
@@ -54204,7 +54094,7 @@
         <v>1774</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>2122</v>
@@ -54218,10 +54108,10 @@
         <v>1774</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>1714</v>
@@ -54232,10 +54122,10 @@
         <v>1774</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>1714</v>
@@ -54246,10 +54136,10 @@
         <v>1774</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="D140" s="9" t="s">
         <v>1719</v>
@@ -54260,10 +54150,10 @@
         <v>1774</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="D141" s="9" t="s">
         <v>1719</v>
@@ -54274,10 +54164,10 @@
         <v>1774</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>1715</v>
@@ -54288,10 +54178,10 @@
         <v>1774</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>1715</v>
@@ -54302,13 +54192,13 @@
         <v>1774</v>
       </c>
       <c r="B144" s="3" t="s">
+        <v>2194</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>2195</v>
       </c>
-      <c r="C144" s="3" t="s">
-        <v>2196</v>
-      </c>
       <c r="D144" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -54316,10 +54206,10 @@
         <v>1774</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>1714</v>
@@ -54330,10 +54220,10 @@
         <v>1774</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>1714</v>
@@ -54344,10 +54234,10 @@
         <v>1774</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>1714</v>
@@ -54358,10 +54248,10 @@
         <v>1774</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>1719</v>
@@ -54372,10 +54262,10 @@
         <v>1774</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>1719</v>
@@ -54391,7 +54281,7 @@
         <v>1774</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>2104</v>
@@ -54405,7 +54295,7 @@
         <v>1774</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>2106</v>
@@ -54419,7 +54309,7 @@
         <v>1774</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>2109</v>
@@ -54433,7 +54323,7 @@
         <v>1774</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>2111</v>
@@ -54447,7 +54337,7 @@
         <v>1774</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>2113</v>
@@ -54461,7 +54351,7 @@
         <v>1774</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>2115</v>
@@ -54475,7 +54365,7 @@
         <v>1774</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>2117</v>
@@ -54489,7 +54379,7 @@
         <v>1774</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>2119</v>
@@ -54503,7 +54393,7 @@
         <v>1774</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>2122</v>
@@ -54517,10 +54407,10 @@
         <v>1774</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>1714</v>
@@ -54531,10 +54421,10 @@
         <v>1774</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>1715</v>
@@ -54545,10 +54435,10 @@
         <v>1774</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>1714</v>
@@ -54559,10 +54449,10 @@
         <v>1774</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>1714</v>
@@ -54573,10 +54463,10 @@
         <v>1774</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>1714</v>
@@ -54587,10 +54477,10 @@
         <v>1774</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>1719</v>
@@ -54601,10 +54491,10 @@
         <v>1774</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>1719</v>
@@ -54615,10 +54505,10 @@
         <v>1774</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>1719</v>
@@ -54629,10 +54519,10 @@
         <v>1774</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>1719</v>
@@ -54648,7 +54538,7 @@
         <v>1774</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>2104</v>
@@ -54662,7 +54552,7 @@
         <v>1774</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>2106</v>
@@ -54676,7 +54566,7 @@
         <v>1774</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>2109</v>
@@ -54690,7 +54580,7 @@
         <v>1774</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>2111</v>
@@ -54704,7 +54594,7 @@
         <v>1774</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>2113</v>
@@ -54718,7 +54608,7 @@
         <v>1774</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>2115</v>
@@ -54732,7 +54622,7 @@
         <v>1774</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>2117</v>
@@ -54746,7 +54636,7 @@
         <v>1774</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>2119</v>
@@ -54760,7 +54650,7 @@
         <v>1774</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>2122</v>
@@ -54774,10 +54664,10 @@
         <v>1774</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>1714</v>
@@ -54788,10 +54678,10 @@
         <v>1774</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>1715</v>
@@ -54802,10 +54692,10 @@
         <v>1774</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>1714</v>
@@ -54816,10 +54706,10 @@
         <v>1774</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>1714</v>
@@ -54830,10 +54720,10 @@
         <v>1774</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>1714</v>
@@ -54844,10 +54734,10 @@
         <v>1774</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>1714</v>
@@ -54858,10 +54748,10 @@
         <v>1774</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>1719</v>
@@ -54872,10 +54762,10 @@
         <v>1774</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>1719</v>
@@ -54891,7 +54781,7 @@
         <v>1774</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>2104</v>
@@ -54905,7 +54795,7 @@
         <v>1774</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>2106</v>
@@ -54919,7 +54809,7 @@
         <v>1774</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>2109</v>
@@ -54933,7 +54823,7 @@
         <v>1774</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>2111</v>
@@ -54947,7 +54837,7 @@
         <v>1774</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>2113</v>
@@ -54961,7 +54851,7 @@
         <v>1774</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>2115</v>
@@ -54975,7 +54865,7 @@
         <v>1774</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>2117</v>
@@ -54989,7 +54879,7 @@
         <v>1774</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>2119</v>
@@ -55003,7 +54893,7 @@
         <v>1774</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>2122</v>
@@ -55017,10 +54907,10 @@
         <v>1774</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>1714</v>
@@ -55031,10 +54921,10 @@
         <v>1774</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>1715</v>
@@ -55045,10 +54935,10 @@
         <v>1774</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>1714</v>
@@ -55059,10 +54949,10 @@
         <v>1774</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>1714</v>
@@ -55073,10 +54963,10 @@
         <v>1774</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>1714</v>
@@ -55087,10 +54977,10 @@
         <v>1774</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>1719</v>
@@ -55101,28 +54991,19 @@
         <v>1774</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>1719</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>2199</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>2302</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>1719</v>
-      </c>
+      <c r="B204" s="3"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
@@ -55132,29 +55013,38 @@
         <v>2199</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>2303</v>
+        <v>2200</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B206" s="3"/>
-      <c r="C206" s="3"/>
-      <c r="D206" s="3"/>
+      <c r="A206" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>2199</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>1715</v>
+      </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>1774</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>2201</v>
+        <v>2109</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -55162,10 +55052,10 @@
         <v>1774</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>2106</v>
+        <v>2111</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>1715</v>
@@ -55176,10 +55066,10 @@
         <v>1774</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>2109</v>
+        <v>2113</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>1715</v>
@@ -55190,13 +55080,13 @@
         <v>1774</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>2111</v>
-      </c>
-      <c r="D210" s="3" t="s">
-        <v>1715</v>
+        <v>2115</v>
+      </c>
+      <c r="D210" s="9" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -55204,13 +55094,13 @@
         <v>1774</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>2113</v>
-      </c>
-      <c r="D211" s="3" t="s">
-        <v>1715</v>
+        <v>2117</v>
+      </c>
+      <c r="D211" s="9" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -55218,12 +55108,12 @@
         <v>1774</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D212" s="9" t="s">
+        <v>2119</v>
+      </c>
+      <c r="D212" s="3" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55232,12 +55122,12 @@
         <v>1774</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="D213" s="9" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D213" s="3" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55246,10 +55136,10 @@
         <v>1774</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>2119</v>
+        <v>2130</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>1714</v>
@@ -55260,10 +55150,10 @@
         <v>1774</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>2122</v>
+        <v>2199</v>
+      </c>
+      <c r="C215" s="9" t="s">
+        <v>2229</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>1714</v>
@@ -55274,10 +55164,10 @@
         <v>1774</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>2131</v>
+        <v>2133</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>1714</v>
@@ -55288,60 +55178,60 @@
         <v>1774</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C217" s="9" t="s">
-        <v>2230</v>
+        <v>2199</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>2135</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>2200</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>2134</v>
-      </c>
-      <c r="D218" s="3" t="s">
-        <v>1714</v>
-      </c>
+      <c r="B218" s="3"/>
+      <c r="C218" s="3"/>
+      <c r="D218" s="3"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>1774</v>
       </c>
       <c r="B219" s="3" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C219" s="3" t="s">
         <v>2200</v>
       </c>
-      <c r="C219" s="3" t="s">
-        <v>2136</v>
-      </c>
       <c r="D219" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B220" s="3"/>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3"/>
+      <c r="A220" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>1715</v>
+      </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>1774</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>2201</v>
+        <v>2109</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -55349,10 +55239,10 @@
         <v>1774</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>2106</v>
+        <v>2111</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>1715</v>
@@ -55363,10 +55253,10 @@
         <v>1774</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>2109</v>
+        <v>2113</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>1715</v>
@@ -55377,13 +55267,13 @@
         <v>1774</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>2111</v>
-      </c>
-      <c r="D224" s="3" t="s">
-        <v>1715</v>
+        <v>2115</v>
+      </c>
+      <c r="D224" s="9" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -55391,13 +55281,13 @@
         <v>1774</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>2113</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>1715</v>
+        <v>2117</v>
+      </c>
+      <c r="D225" s="9" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -55405,12 +55295,12 @@
         <v>1774</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D226" s="9" t="s">
+        <v>2119</v>
+      </c>
+      <c r="D226" s="3" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55419,12 +55309,12 @@
         <v>1774</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="D227" s="9" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D227" s="3" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55433,10 +55323,10 @@
         <v>1774</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>2119</v>
+        <v>2149</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>1714</v>
@@ -55447,13 +55337,13 @@
         <v>1774</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>2122</v>
+        <v>2151</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -55461,10 +55351,10 @@
         <v>1774</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>2150</v>
+        <v>2130</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>1714</v>
@@ -55475,13 +55365,13 @@
         <v>1774</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>2202</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>2152</v>
+        <v>2201</v>
+      </c>
+      <c r="C231" s="9" t="s">
+        <v>2229</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -55489,10 +55379,10 @@
         <v>1774</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>2131</v>
+        <v>2133</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>1714</v>
@@ -55503,13 +55393,13 @@
         <v>1774</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>2202</v>
-      </c>
-      <c r="C233" s="9" t="s">
-        <v>2230</v>
+        <v>2201</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>2135</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -55517,41 +55407,41 @@
         <v>1774</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>2134</v>
+        <v>2216</v>
       </c>
       <c r="D234" s="3" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B236" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C236" s="14" t="s">
+        <v>2104</v>
+      </c>
+      <c r="D236" s="14" t="s">
         <v>1714</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" t="s">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="14" t="s">
         <v>1774</v>
       </c>
-      <c r="B235" s="3" t="s">
-        <v>2202</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>2136</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B236" s="3" t="s">
-        <v>2202</v>
-      </c>
-      <c r="C236" s="3" t="s">
-        <v>2217</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>1719</v>
+      <c r="B237" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C237" s="14" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D237" s="14" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -55559,13 +55449,13 @@
         <v>1774</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C238" s="14" t="s">
-        <v>2104</v>
+        <v>2109</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
@@ -55573,10 +55463,10 @@
         <v>1774</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C239" s="14" t="s">
-        <v>2106</v>
+        <v>2111</v>
       </c>
       <c r="D239" s="14" t="s">
         <v>1715</v>
@@ -55587,10 +55477,10 @@
         <v>1774</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>2109</v>
+        <v>2113</v>
       </c>
       <c r="D240" s="14" t="s">
         <v>1715</v>
@@ -55601,13 +55491,13 @@
         <v>1774</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>2111</v>
+        <v>2115</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -55615,13 +55505,13 @@
         <v>1774</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>2113</v>
+        <v>2117</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -55629,10 +55519,10 @@
         <v>1774</v>
       </c>
       <c r="B243" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>2115</v>
+        <v>2119</v>
       </c>
       <c r="D243" s="14" t="s">
         <v>1714</v>
@@ -55643,10 +55533,10 @@
         <v>1774</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>2117</v>
+        <v>2122</v>
       </c>
       <c r="D244" s="14" t="s">
         <v>1714</v>
@@ -55657,10 +55547,10 @@
         <v>1774</v>
       </c>
       <c r="B245" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>2119</v>
+        <v>2139</v>
       </c>
       <c r="D245" s="14" t="s">
         <v>1714</v>
@@ -55671,10 +55561,10 @@
         <v>1774</v>
       </c>
       <c r="B246" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C246" s="14" t="s">
-        <v>2122</v>
+        <v>2141</v>
       </c>
       <c r="D246" s="14" t="s">
         <v>1714</v>
@@ -55685,13 +55575,13 @@
         <v>1774</v>
       </c>
       <c r="B247" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C247" s="14" t="s">
-        <v>2140</v>
-      </c>
-      <c r="D247" s="14" t="s">
-        <v>1714</v>
+        <v>2145</v>
+      </c>
+      <c r="D247" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -55699,13 +55589,13 @@
         <v>1774</v>
       </c>
       <c r="B248" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C248" s="14" t="s">
-        <v>2142</v>
-      </c>
-      <c r="D248" s="14" t="s">
-        <v>1714</v>
+        <v>2147</v>
+      </c>
+      <c r="D248" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -55713,13 +55603,13 @@
         <v>1774</v>
       </c>
       <c r="B249" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C249" s="14" t="s">
-        <v>2146</v>
-      </c>
-      <c r="D249" s="9" t="s">
-        <v>1719</v>
+        <v>2137</v>
+      </c>
+      <c r="D249" s="14" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -55727,13 +55617,13 @@
         <v>1774</v>
       </c>
       <c r="B250" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C250" s="14" t="s">
-        <v>2148</v>
-      </c>
-      <c r="D250" s="9" t="s">
-        <v>1719</v>
+        <v>2138</v>
+      </c>
+      <c r="D250" s="14" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
@@ -55741,13 +55631,13 @@
         <v>1774</v>
       </c>
       <c r="B251" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C251" s="14" t="s">
-        <v>2138</v>
+        <v>2130</v>
       </c>
       <c r="D251" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
@@ -55755,13 +55645,13 @@
         <v>1774</v>
       </c>
       <c r="B252" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C252" s="14" t="s">
-        <v>2139</v>
+        <v>2229</v>
       </c>
       <c r="D252" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
@@ -55769,10 +55659,10 @@
         <v>1774</v>
       </c>
       <c r="B253" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C253" s="14" t="s">
-        <v>2131</v>
+        <v>2133</v>
       </c>
       <c r="D253" s="14" t="s">
         <v>1714</v>
@@ -55783,13 +55673,13 @@
         <v>1774</v>
       </c>
       <c r="B254" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C254" s="14" t="s">
-        <v>2230</v>
+        <v>2135</v>
       </c>
       <c r="D254" s="14" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
@@ -55797,40 +55687,12 @@
         <v>1774</v>
       </c>
       <c r="B255" s="14" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="C255" s="14" t="s">
-        <v>2134</v>
+        <v>2216</v>
       </c>
       <c r="D255" s="14" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A256" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B256" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="C256" s="14" t="s">
-        <v>2136</v>
-      </c>
-      <c r="D256" s="14" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A257" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B257" s="14" t="s">
-        <v>2262</v>
-      </c>
-      <c r="C257" s="14" t="s">
-        <v>2217</v>
-      </c>
-      <c r="D257" s="14" t="s">
         <v>1719</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated metadata sheet for NGID
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdaws/Documents/fairds_storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF39E4B-4721-3543-9034-E5009C63AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653DE535-2B82-9646-AD17-269D5DC0675E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regex" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13612" uniqueCount="2301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13661" uniqueCount="2313">
   <si>
     <t>short hand form</t>
   </si>
@@ -7097,6 +7097,42 @@
   </si>
   <si>
     <t>({text}{1,3}/{text}{1,3}|unknown)</t>
+  </si>
+  <si>
+    <t>ethnicity</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>fitzpatrick</t>
+  </si>
+  <si>
+    <t>Specific to psoriasis data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treatment administered to patient </t>
+  </si>
+  <si>
+    <t>a classification system that categorizes skin based on its reaction to sun exposure, specifically its tendency to burn or tan</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16564</t>
+  </si>
+  <si>
+    <t>A social group characterized by a distinctive social and cultural tradition that is maintained from generation to generation.</t>
+  </si>
+  <si>
+    <t>recimmended</t>
+  </si>
+  <si>
+    <t>labnotes</t>
+  </si>
+  <si>
+    <t>location of labnotes</t>
+  </si>
+  <si>
+    <t>location of additional comments on sample preparation/analysis</t>
   </si>
 </sst>
 </file>
@@ -7909,11 +7945,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F772"/>
+  <dimension ref="A1:F777"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A685" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B689" sqref="B689"/>
+      <pane ySplit="1" topLeftCell="A733" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F745" sqref="F745"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16823,444 +16859,509 @@
         <v>2290</v>
       </c>
     </row>
+    <row r="735" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A735" s="3" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B735" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E735" s="2"/>
+      <c r="F735" s="3" t="s">
+        <v>2305</v>
+      </c>
+    </row>
     <row r="736" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A736" s="3" t="s">
-        <v>2176</v>
+        <v>2303</v>
       </c>
       <c r="B736" s="3" t="s">
-        <v>2157</v>
-      </c>
-      <c r="C736" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E736" s="3" t="s">
-        <v>194</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="E736" s="2"/>
       <c r="F736" s="3" t="s">
-        <v>2176</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="737" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A737" s="3" t="s">
-        <v>2177</v>
-      </c>
-      <c r="B737" s="3" t="s">
-        <v>2157</v>
-      </c>
-      <c r="C737" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E737" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F737" s="3" t="s">
-        <v>2178</v>
+        <v>2301</v>
+      </c>
+      <c r="B737" t="s">
+        <v>241</v>
+      </c>
+      <c r="E737" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F737" t="s">
+        <v>2308</v>
       </c>
     </row>
     <row r="738" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A738" s="3" t="s">
-        <v>2206</v>
+        <v>2176</v>
       </c>
       <c r="B738" s="3" t="s">
-        <v>2179</v>
+        <v>2157</v>
       </c>
       <c r="C738" s="3" t="s">
-        <v>2180</v>
-      </c>
-      <c r="E738" s="3"/>
+        <v>245</v>
+      </c>
+      <c r="E738" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="F738" s="3" t="s">
-        <v>2181</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A739" s="3" t="s">
-        <v>2182</v>
+        <v>2177</v>
       </c>
       <c r="B739" s="3" t="s">
-        <v>847</v>
+        <v>2157</v>
       </c>
       <c r="C739" s="3" t="s">
-        <v>1408</v>
-      </c>
-      <c r="E739" s="2" t="s">
-        <v>2205</v>
+        <v>245</v>
+      </c>
+      <c r="E739" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="F739" s="3" t="s">
-        <v>2183</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="740" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A740" s="3" t="s">
-        <v>2184</v>
+        <v>2206</v>
       </c>
       <c r="B740" s="3" t="s">
-        <v>2215</v>
+        <v>2179</v>
       </c>
       <c r="C740" s="3" t="s">
-        <v>2185</v>
+        <v>2180</v>
       </c>
       <c r="E740" s="3"/>
       <c r="F740" s="3" t="s">
-        <v>2186</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="741" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A741" s="3" t="s">
-        <v>2187</v>
+        <v>2182</v>
       </c>
       <c r="B741" s="3" t="s">
-        <v>73</v>
+        <v>847</v>
       </c>
       <c r="C741" s="3" t="s">
-        <v>2188</v>
-      </c>
-      <c r="E741" s="3"/>
+        <v>1408</v>
+      </c>
+      <c r="E741" s="2" t="s">
+        <v>2205</v>
+      </c>
       <c r="F741" s="3" t="s">
-        <v>2189</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A742" s="3" t="s">
-        <v>2207</v>
+        <v>2184</v>
       </c>
       <c r="B742" s="3" t="s">
-        <v>2214</v>
-      </c>
-      <c r="C742">
-        <v>1993</v>
-      </c>
+        <v>2215</v>
+      </c>
+      <c r="C742" s="3" t="s">
+        <v>2185</v>
+      </c>
+      <c r="E742" s="3"/>
       <c r="F742" s="3" t="s">
-        <v>2207</v>
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="743" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A743" s="3" t="s">
+        <v>2187</v>
+      </c>
+      <c r="B743" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C743" s="3" t="s">
+        <v>2188</v>
+      </c>
+      <c r="E743" s="3"/>
+      <c r="F743" s="3" t="s">
+        <v>2189</v>
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A744" s="3" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="B744" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C744" s="3" t="s">
-        <v>2209</v>
+        <v>2214</v>
+      </c>
+      <c r="C744">
+        <v>1993</v>
+      </c>
+      <c r="F744" s="3" t="s">
+        <v>2207</v>
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A745" s="3" t="s">
-        <v>2210</v>
+        <v>1055</v>
       </c>
       <c r="B745" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C745">
-        <v>25</v>
+        <v>73</v>
+      </c>
+      <c r="F745" s="3" t="s">
+        <v>2312</v>
       </c>
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A746" s="3" t="s">
-        <v>2211</v>
+        <v>2310</v>
       </c>
       <c r="B746" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C746" t="s">
-        <v>2212</v>
-      </c>
-      <c r="F746" t="s">
-        <v>2213</v>
-      </c>
-    </row>
-    <row r="748" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A748" s="3" t="s">
-        <v>2216</v>
-      </c>
-      <c r="B748" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F746" s="3" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="747" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A747" s="3"/>
+      <c r="B747" s="3"/>
+      <c r="F747" s="3"/>
     </row>
     <row r="749" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A749" s="3" t="s">
-        <v>2218</v>
+        <v>2208</v>
       </c>
       <c r="B749" s="3" t="s">
-        <v>2220</v>
-      </c>
-      <c r="C749" t="s">
-        <v>2222</v>
+        <v>10</v>
+      </c>
+      <c r="C749" s="3" t="s">
+        <v>2209</v>
       </c>
     </row>
     <row r="750" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A750" s="3" t="s">
-        <v>2262</v>
+        <v>2210</v>
       </c>
       <c r="B750" s="3" t="s">
-        <v>2277</v>
+        <v>28</v>
+      </c>
+      <c r="C750">
+        <v>25</v>
       </c>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A751" s="3" t="s">
-        <v>2263</v>
+        <v>2211</v>
       </c>
       <c r="B751" s="3" t="s">
-        <v>2278</v>
-      </c>
-    </row>
-    <row r="752" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A752" s="3" t="s">
-        <v>2219</v>
-      </c>
-      <c r="B752" s="3" t="s">
-        <v>2221</v>
-      </c>
-      <c r="C752" t="s">
-        <v>2223</v>
-      </c>
-    </row>
-    <row r="753" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C751" t="s">
+        <v>2212</v>
+      </c>
+      <c r="F751" t="s">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A753" s="3" t="s">
-        <v>2264</v>
+        <v>2216</v>
       </c>
       <c r="B753" s="3" t="s">
-        <v>2276</v>
-      </c>
-      <c r="E753" s="15" t="s">
-        <v>2265</v>
+        <v>10</v>
       </c>
     </row>
     <row r="754" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A754" s="3" t="s">
-        <v>2224</v>
+        <v>2218</v>
       </c>
       <c r="B754" s="3" t="s">
-        <v>50</v>
+        <v>2220</v>
+      </c>
+      <c r="C754" t="s">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A755" s="3" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B755" s="3" t="s">
+        <v>2277</v>
       </c>
     </row>
     <row r="756" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A756" s="3" t="s">
-        <v>2226</v>
+        <v>2263</v>
       </c>
       <c r="B756" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C756" t="s">
-        <v>2258</v>
-      </c>
-      <c r="E756" s="12" t="s">
-        <v>2259</v>
-      </c>
-      <c r="F756" t="s">
-        <v>2227</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="757" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A757" s="3" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B757" s="3" t="s">
+        <v>2221</v>
+      </c>
+      <c r="C757" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="758" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A758" s="3" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B758" s="3" t="s">
+        <v>2276</v>
+      </c>
+      <c r="E758" s="15" t="s">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="759" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A759" s="3" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B759" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A761" s="3" t="s">
+        <v>2226</v>
+      </c>
+      <c r="B761" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C761" t="s">
+        <v>2258</v>
+      </c>
+      <c r="E761" s="12" t="s">
+        <v>2259</v>
+      </c>
+      <c r="F761" t="s">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A762" s="3" t="s">
         <v>2228</v>
       </c>
-      <c r="B757" s="3" t="s">
+      <c r="B762" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="758" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A758" s="3" t="s">
+    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A763" s="3" t="s">
         <v>2230</v>
       </c>
-      <c r="B758" s="3" t="s">
+      <c r="B763" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C758" t="s">
+      <c r="C763" t="s">
         <v>1231</v>
       </c>
-      <c r="E758" t="s">
+      <c r="E763" t="s">
         <v>2231</v>
-      </c>
-    </row>
-    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A760" s="10" t="s">
-        <v>2260</v>
-      </c>
-      <c r="B760" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C760" s="13" t="s">
-        <v>2254</v>
-      </c>
-      <c r="E760" s="12" t="s">
-        <v>2266</v>
-      </c>
-      <c r="F760" s="11" t="s">
-        <v>2243</v>
-      </c>
-    </row>
-    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A761" s="10" t="s">
-        <v>2233</v>
-      </c>
-      <c r="B761" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C761" s="13" t="s">
-        <v>2255</v>
-      </c>
-      <c r="E761" s="12" t="s">
-        <v>2275</v>
-      </c>
-      <c r="F761" t="s">
-        <v>2244</v>
-      </c>
-    </row>
-    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A762" s="10" t="s">
-        <v>2234</v>
-      </c>
-      <c r="B762" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C762" s="13" t="s">
-        <v>2256</v>
-      </c>
-      <c r="E762" s="12" t="s">
-        <v>2274</v>
-      </c>
-      <c r="F762" t="s">
-        <v>2245</v>
-      </c>
-    </row>
-    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A763" s="10" t="s">
-        <v>2235</v>
-      </c>
-      <c r="B763" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C763" s="13" t="s">
-        <v>2257</v>
-      </c>
-      <c r="E763" s="12" t="s">
-        <v>2269</v>
-      </c>
-      <c r="F763" t="s">
-        <v>2246</v>
-      </c>
-    </row>
-    <row r="764" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A764" s="10" t="s">
-        <v>2236</v>
-      </c>
-      <c r="B764" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C764" s="13" t="s">
-        <v>2279</v>
-      </c>
-      <c r="E764" s="12" t="s">
-        <v>2267</v>
-      </c>
-      <c r="F764" t="s">
-        <v>2247</v>
       </c>
     </row>
     <row r="765" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A765" s="10" t="s">
-        <v>2237</v>
+        <v>2260</v>
       </c>
       <c r="B765" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C765" s="13" t="s">
-        <v>2280</v>
+        <v>2254</v>
       </c>
       <c r="E765" s="12" t="s">
-        <v>2268</v>
-      </c>
-      <c r="F765" t="s">
-        <v>2248</v>
+        <v>2266</v>
+      </c>
+      <c r="F765" s="11" t="s">
+        <v>2243</v>
       </c>
     </row>
     <row r="766" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A766" s="10" t="s">
-        <v>2238</v>
+        <v>2233</v>
       </c>
       <c r="B766" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C766" s="13" t="s">
-        <v>2281</v>
+        <v>2255</v>
       </c>
       <c r="E766" s="12" t="s">
-        <v>2271</v>
+        <v>2275</v>
       </c>
       <c r="F766" t="s">
-        <v>2249</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="767" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A767" s="10" t="s">
-        <v>2239</v>
+        <v>2234</v>
       </c>
       <c r="B767" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C767" s="13" t="s">
-        <v>2282</v>
+        <v>2256</v>
       </c>
       <c r="E767" s="12" t="s">
-        <v>2272</v>
+        <v>2274</v>
       </c>
       <c r="F767" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="768" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A768" s="10" t="s">
-        <v>2240</v>
+        <v>2235</v>
       </c>
       <c r="B768" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C768" s="13" t="s">
-        <v>2283</v>
-      </c>
-      <c r="E768" s="12"/>
+        <v>2257</v>
+      </c>
+      <c r="E768" s="12" t="s">
+        <v>2269</v>
+      </c>
       <c r="F768" t="s">
-        <v>2251</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="769" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A769" s="10" t="s">
-        <v>2241</v>
+        <v>2236</v>
       </c>
       <c r="B769" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C769" s="13" t="s">
-        <v>2284</v>
+        <v>2279</v>
       </c>
       <c r="E769" s="12" t="s">
-        <v>2273</v>
+        <v>2267</v>
       </c>
       <c r="F769" t="s">
-        <v>2252</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="770" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A770" s="10" t="s">
-        <v>2242</v>
+        <v>2237</v>
       </c>
       <c r="B770" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C770" s="13" t="s">
+        <v>2280</v>
+      </c>
+      <c r="E770" s="12" t="s">
+        <v>2268</v>
+      </c>
+      <c r="F770" t="s">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="771" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A771" s="10" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B771" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C771" s="13" t="s">
+        <v>2281</v>
+      </c>
+      <c r="E771" s="12" t="s">
+        <v>2271</v>
+      </c>
+      <c r="F771" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A772" s="10" t="s">
+        <v>2239</v>
+      </c>
+      <c r="B772" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C772" s="13" t="s">
+        <v>2282</v>
+      </c>
+      <c r="E772" s="12" t="s">
+        <v>2272</v>
+      </c>
+      <c r="F772" t="s">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="773" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A773" s="10" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B773" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C773" s="13" t="s">
+        <v>2283</v>
+      </c>
+      <c r="E773" s="12"/>
+      <c r="F773" t="s">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="774" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A774" s="10" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B774" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C774" s="13" t="s">
+        <v>2284</v>
+      </c>
+      <c r="E774" s="12" t="s">
+        <v>2273</v>
+      </c>
+      <c r="F774" t="s">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="775" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A775" s="10" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B775" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C775" s="13" t="s">
         <v>2255</v>
       </c>
-      <c r="E770" s="12" t="s">
+      <c r="E775" s="12" t="s">
         <v>2270</v>
       </c>
-      <c r="F770" t="s">
+      <c r="F775" t="s">
         <v>2253</v>
       </c>
     </row>
-    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A772" s="10"/>
-      <c r="B772" s="3"/>
+    <row r="777" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A777" s="10"/>
+      <c r="B777" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -17268,8 +17369,8 @@
     <hyperlink ref="E11" r:id="rId1" display="https://w3id.org/mixs/terms/0000018" xr:uid="{E5B9998C-031F-4241-A1E7-C7E6D8677047}"/>
     <hyperlink ref="E559" r:id="rId2" xr:uid="{EC998EC6-084C-3048-AC10-E9220B7375C6}"/>
     <hyperlink ref="C730" r:id="rId3" xr:uid="{52CD8FE2-FCDC-D545-943E-8E5695A7E4C6}"/>
-    <hyperlink ref="E739" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
-    <hyperlink ref="E756" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
+    <hyperlink ref="E741" r:id="rId4" xr:uid="{3E1D9C48-AD95-9E43-81EC-742699861080}"/>
+    <hyperlink ref="E761" r:id="rId5" xr:uid="{D214A32F-7CBA-8B4B-B83C-E607FA5207D8}"/>
     <hyperlink ref="E734" r:id="rId6" xr:uid="{02045287-A2C1-2246-9C9A-09E35261DF8C}"/>
     <hyperlink ref="E733" r:id="rId7" xr:uid="{0FD7D99F-B07A-9643-9AD4-E0FEFB759009}"/>
     <hyperlink ref="E724" r:id="rId8" xr:uid="{383BC27E-9C9C-494A-88BF-6F6240C62D83}"/>
@@ -17519,10 +17620,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17972,7 +18073,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>1717</v>
       </c>
@@ -17986,7 +18087,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18000,7 +18101,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18014,7 +18115,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18025,10 +18126,10 @@
         <v>2207</v>
       </c>
       <c r="D38" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18042,7 +18143,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18056,7 +18157,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18070,7 +18171,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18084,7 +18185,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18098,7 +18199,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>1717</v>
       </c>
@@ -18109,6 +18210,65 @@
         <v>2187</v>
       </c>
       <c r="D44" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>2301</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>2303</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D48" t="s">
         <v>1719</v>
       </c>
     </row>
@@ -52373,10 +52533,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D255"/>
+  <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54614,7 +54774,7 @@
         <v>2115</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -54628,7 +54788,7 @@
         <v>2117</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -54642,7 +54802,7 @@
         <v>2119</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -54656,7 +54816,7 @@
         <v>2122</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -54726,7 +54886,7 @@
         <v>2295</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -54772,37 +54932,37 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
+      <c r="A187" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>2197</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>1719</v>
+      </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>1774</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>2104</v>
+        <v>2310</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>1714</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>2198</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>2106</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>1715</v>
-      </c>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="3"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
@@ -54812,10 +54972,10 @@
         <v>2198</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>2109</v>
+        <v>2104</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -54826,7 +54986,7 @@
         <v>2198</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>1715</v>
@@ -54840,7 +55000,7 @@
         <v>2198</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>2113</v>
+        <v>2109</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>1715</v>
@@ -54854,10 +55014,10 @@
         <v>2198</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>1714</v>
+        <v>2111</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -54868,10 +55028,10 @@
         <v>2198</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="D194" s="9" t="s">
-        <v>1714</v>
+        <v>2113</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -54882,10 +55042,10 @@
         <v>2198</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>2119</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>1714</v>
+        <v>2115</v>
+      </c>
+      <c r="D195" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -54896,10 +55056,10 @@
         <v>2198</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>2122</v>
-      </c>
-      <c r="D196" s="3" t="s">
-        <v>1714</v>
+        <v>2117</v>
+      </c>
+      <c r="D196" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -54910,10 +55070,10 @@
         <v>2198</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>2149</v>
+        <v>2119</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -54924,7 +55084,7 @@
         <v>2198</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>2151</v>
+        <v>2122</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>1715</v>
@@ -54938,7 +55098,7 @@
         <v>2198</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>2130</v>
+        <v>2149</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>1714</v>
@@ -54951,11 +55111,11 @@
       <c r="B200" s="3" t="s">
         <v>2198</v>
       </c>
-      <c r="C200" s="9" t="s">
-        <v>2229</v>
+      <c r="C200" s="3" t="s">
+        <v>2151</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -54966,7 +55126,7 @@
         <v>2198</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>1714</v>
@@ -54979,11 +55139,11 @@
       <c r="B202" s="3" t="s">
         <v>2198</v>
       </c>
-      <c r="C202" s="3" t="s">
-        <v>2135</v>
+      <c r="C202" s="9" t="s">
+        <v>2229</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -54994,29 +55154,38 @@
         <v>2198</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>2216</v>
+        <v>2133</v>
       </c>
       <c r="D203" s="3" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>2198</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D204" s="3" t="s">
         <v>1719</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B204" s="3"/>
-      <c r="C204" s="3"/>
-      <c r="D204" s="3"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>1774</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>2200</v>
+        <v>2216</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>1714</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -55024,13 +55193,13 @@
         <v>1774</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>2106</v>
+        <v>1055</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>1715</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
@@ -55038,28 +55207,19 @@
         <v>1774</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>2109</v>
+        <v>2310</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>1715</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>2199</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>2111</v>
-      </c>
-      <c r="D208" s="3" t="s">
-        <v>1715</v>
-      </c>
+      <c r="B208" s="3"/>
+      <c r="C208" s="3"/>
+      <c r="D208" s="3"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
@@ -55069,10 +55229,10 @@
         <v>2199</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>2113</v>
+        <v>2200</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -55083,10 +55243,10 @@
         <v>2199</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D210" s="9" t="s">
-        <v>1714</v>
+        <v>2106</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -55097,10 +55257,10 @@
         <v>2199</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="D211" s="9" t="s">
-        <v>1714</v>
+        <v>2109</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -55111,10 +55271,10 @@
         <v>2199</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>2119</v>
+        <v>2111</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
@@ -55125,10 +55285,10 @@
         <v>2199</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>2122</v>
+        <v>2113</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -55139,9 +55299,9 @@
         <v>2199</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>2130</v>
-      </c>
-      <c r="D214" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="D214" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55152,10 +55312,10 @@
       <c r="B215" s="3" t="s">
         <v>2199</v>
       </c>
-      <c r="C215" s="9" t="s">
-        <v>2229</v>
-      </c>
-      <c r="D215" s="3" t="s">
+      <c r="C215" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D215" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55167,7 +55327,7 @@
         <v>2199</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>2133</v>
+        <v>2119</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>1714</v>
@@ -55181,26 +55341,35 @@
         <v>2199</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>2135</v>
+        <v>2122</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B218" s="3"/>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3"/>
+      <c r="A218" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>2199</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>1714</v>
+      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>1774</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>2201</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
+      </c>
+      <c r="C219" s="9" t="s">
+        <v>2229</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>1714</v>
@@ -55211,13 +55380,13 @@
         <v>1774</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>2106</v>
+        <v>2133</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -55225,28 +55394,19 @@
         <v>1774</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>2109</v>
+        <v>2135</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>1715</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B222" s="3" t="s">
-        <v>2201</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>2111</v>
-      </c>
-      <c r="D222" s="3" t="s">
-        <v>1715</v>
-      </c>
+      <c r="B222" s="3"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="3"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
@@ -55256,10 +55416,10 @@
         <v>2201</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>2113</v>
+        <v>2200</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -55270,10 +55430,10 @@
         <v>2201</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>2115</v>
-      </c>
-      <c r="D224" s="9" t="s">
-        <v>1714</v>
+        <v>2106</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -55284,10 +55444,10 @@
         <v>2201</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>2117</v>
-      </c>
-      <c r="D225" s="9" t="s">
-        <v>1714</v>
+        <v>2109</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>1715</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -55298,10 +55458,10 @@
         <v>2201</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>2119</v>
+        <v>2111</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -55312,10 +55472,10 @@
         <v>2201</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>2122</v>
+        <v>2113</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -55326,9 +55486,9 @@
         <v>2201</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>2149</v>
-      </c>
-      <c r="D228" s="3" t="s">
+        <v>2115</v>
+      </c>
+      <c r="D228" s="9" t="s">
         <v>1714</v>
       </c>
     </row>
@@ -55340,10 +55500,10 @@
         <v>2201</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>2151</v>
-      </c>
-      <c r="D229" s="3" t="s">
-        <v>1715</v>
+        <v>2117</v>
+      </c>
+      <c r="D229" s="9" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -55354,7 +55514,7 @@
         <v>2201</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>2130</v>
+        <v>2119</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>1714</v>
@@ -55367,8 +55527,8 @@
       <c r="B231" s="3" t="s">
         <v>2201</v>
       </c>
-      <c r="C231" s="9" t="s">
-        <v>2229</v>
+      <c r="C231" s="3" t="s">
+        <v>2122</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>1714</v>
@@ -55382,7 +55542,7 @@
         <v>2201</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>2133</v>
+        <v>2149</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>1714</v>
@@ -55396,10 +55556,10 @@
         <v>2201</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>2135</v>
+        <v>2151</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>1719</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -55410,66 +55570,66 @@
         <v>2201</v>
       </c>
       <c r="C234" s="3" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C235" s="9" t="s">
+        <v>2229</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>2133</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C238" s="3" t="s">
         <v>2216</v>
       </c>
-      <c r="D234" s="3" t="s">
+      <c r="D238" s="3" t="s">
         <v>1719</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B236" s="14" t="s">
-        <v>2261</v>
-      </c>
-      <c r="C236" s="14" t="s">
-        <v>2104</v>
-      </c>
-      <c r="D236" s="14" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A237" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B237" s="14" t="s">
-        <v>2261</v>
-      </c>
-      <c r="C237" s="14" t="s">
-        <v>2106</v>
-      </c>
-      <c r="D237" s="14" t="s">
-        <v>1715</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A238" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B238" s="14" t="s">
-        <v>2261</v>
-      </c>
-      <c r="C238" s="14" t="s">
-        <v>2109</v>
-      </c>
-      <c r="D238" s="14" t="s">
-        <v>1715</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="14" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B239" s="14" t="s">
-        <v>2261</v>
-      </c>
-      <c r="C239" s="14" t="s">
-        <v>2111</v>
-      </c>
-      <c r="D239" s="14" t="s">
-        <v>1715</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -55480,10 +55640,10 @@
         <v>2261</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>2113</v>
+        <v>2104</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -55494,10 +55654,10 @@
         <v>2261</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>2115</v>
+        <v>2106</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -55508,10 +55668,10 @@
         <v>2261</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>2117</v>
+        <v>2109</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -55522,10 +55682,10 @@
         <v>2261</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>2119</v>
+        <v>2111</v>
       </c>
       <c r="D243" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
@@ -55536,10 +55696,10 @@
         <v>2261</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>2122</v>
+        <v>2113</v>
       </c>
       <c r="D244" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
@@ -55550,7 +55710,7 @@
         <v>2261</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>2139</v>
+        <v>2115</v>
       </c>
       <c r="D245" s="14" t="s">
         <v>1714</v>
@@ -55564,7 +55724,7 @@
         <v>2261</v>
       </c>
       <c r="C246" s="14" t="s">
-        <v>2141</v>
+        <v>2117</v>
       </c>
       <c r="D246" s="14" t="s">
         <v>1714</v>
@@ -55578,10 +55738,10 @@
         <v>2261</v>
       </c>
       <c r="C247" s="14" t="s">
-        <v>2145</v>
-      </c>
-      <c r="D247" s="9" t="s">
-        <v>1719</v>
+        <v>2119</v>
+      </c>
+      <c r="D247" s="14" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -55592,10 +55752,10 @@
         <v>2261</v>
       </c>
       <c r="C248" s="14" t="s">
-        <v>2147</v>
-      </c>
-      <c r="D248" s="9" t="s">
-        <v>1719</v>
+        <v>2122</v>
+      </c>
+      <c r="D248" s="14" t="s">
+        <v>1714</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -55606,10 +55766,10 @@
         <v>2261</v>
       </c>
       <c r="C249" s="14" t="s">
-        <v>2137</v>
+        <v>2139</v>
       </c>
       <c r="D249" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -55620,10 +55780,10 @@
         <v>2261</v>
       </c>
       <c r="C250" s="14" t="s">
-        <v>2138</v>
+        <v>2141</v>
       </c>
       <c r="D250" s="14" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
@@ -55634,10 +55794,10 @@
         <v>2261</v>
       </c>
       <c r="C251" s="14" t="s">
-        <v>2130</v>
-      </c>
-      <c r="D251" s="14" t="s">
-        <v>1714</v>
+        <v>2145</v>
+      </c>
+      <c r="D251" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
@@ -55648,10 +55808,10 @@
         <v>2261</v>
       </c>
       <c r="C252" s="14" t="s">
-        <v>2229</v>
-      </c>
-      <c r="D252" s="14" t="s">
-        <v>1714</v>
+        <v>2147</v>
+      </c>
+      <c r="D252" s="9" t="s">
+        <v>1719</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
@@ -55662,10 +55822,10 @@
         <v>2261</v>
       </c>
       <c r="C253" s="14" t="s">
-        <v>2133</v>
+        <v>2137</v>
       </c>
       <c r="D253" s="14" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
@@ -55676,10 +55836,10 @@
         <v>2261</v>
       </c>
       <c r="C254" s="14" t="s">
-        <v>2135</v>
+        <v>2138</v>
       </c>
       <c r="D254" s="14" t="s">
-        <v>1719</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
@@ -55690,9 +55850,65 @@
         <v>2261</v>
       </c>
       <c r="C255" s="14" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D255" s="14" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B256" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C256" s="14" t="s">
+        <v>2229</v>
+      </c>
+      <c r="D256" s="14" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B257" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C257" s="14" t="s">
+        <v>2133</v>
+      </c>
+      <c r="D257" s="14" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B258" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C258" s="14" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D258" s="14" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B259" s="14" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C259" s="14" t="s">
         <v>2216</v>
       </c>
-      <c r="D255" s="14" t="s">
+      <c r="D259" s="14" t="s">
         <v>1719</v>
       </c>
     </row>

</xml_diff>